<commit_message>
Revisión escaleta guion 7
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/Escaleta_LE_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/Escaleta_LE_08_07_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="330">
   <si>
     <t>Asignatura</t>
   </si>
@@ -482,15 +482,6 @@
     <t>Escribe un ensayo</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: el ensayo</t>
-  </si>
-  <si>
-    <t>Producción textual: Ordena los argumentos de un ensayo</t>
-  </si>
-  <si>
-    <t>Banco de actividades: El ensayo</t>
-  </si>
-  <si>
     <t>Mapa conceptual del tema El ensayo</t>
   </si>
   <si>
@@ -527,12 +518,6 @@
     <t>LC_10_10</t>
   </si>
   <si>
-    <t>Interactivo que sirve para esquematizar los pasos a realizar en el análisis de oraciones compuestas</t>
-  </si>
-  <si>
-    <t>Identifica los nexos de las oraciones compuestas</t>
-  </si>
-  <si>
     <t>Los medios de comunicación</t>
   </si>
   <si>
@@ -557,9 +542,6 @@
     <t>LC_09_18</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Identifica el tipo de oración compuesta</t>
-  </si>
-  <si>
     <t>La literatura medieval</t>
   </si>
   <si>
@@ -569,9 +551,6 @@
     <t>LC_09_04</t>
   </si>
   <si>
-    <t>Actividad para analizar e identificar el tipo de oración compuesta</t>
-  </si>
-  <si>
     <t>Ordena oraciones compuestas según nexos y signos de puntuación</t>
   </si>
   <si>
@@ -581,9 +560,6 @@
     <t>El paréntesis, el guion y la raya</t>
   </si>
   <si>
-    <t>Interactivo que expone el uso de lo signos de puntuación</t>
-  </si>
-  <si>
     <t>La ortografía</t>
   </si>
   <si>
@@ -593,15 +569,6 @@
     <t>Practica los usos del paréntesis, del guion y la raya</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Practica los usos del paréntesis, del guion y la raya</t>
-  </si>
-  <si>
-    <t>Actividad para practicar el uso correcto de los signos de puntuación</t>
-  </si>
-  <si>
-    <t>Ortografía: Define algunos signos de puntuación</t>
-  </si>
-  <si>
     <t>El reportaje</t>
   </si>
   <si>
@@ -614,9 +581,6 @@
     <t xml:space="preserve">Revisar el recurso y ajustar el vocabulario y el lenguaje a nuestro contexto. Si considera pertinente ampliarlo lo puede hacer. Remplazar la definición de comillas por el signo faltante de acuerdo al tema visto. </t>
   </si>
   <si>
-    <t>Actividad para distinguir los signos de puntuación</t>
-  </si>
-  <si>
     <t>Los textos formales</t>
   </si>
   <si>
@@ -626,9 +590,6 @@
     <t>LC_09_25</t>
   </si>
   <si>
-    <t>Interactivo que estudia paso a paso las características que presenta un ensayo</t>
-  </si>
-  <si>
     <t>Ordena las intervenciones de los personajes</t>
   </si>
   <si>
@@ -641,62 +602,357 @@
     <t>LC_08_11</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad para identificar el estilo de Márquez </t>
-  </si>
-  <si>
     <t>5 oraciones compuestas para completar, relacionadas con el tema literario visto.</t>
   </si>
   <si>
-    <t>Ortografía: los signos de puntuación</t>
-  </si>
-  <si>
-    <t>Actividad para repasar los nexos que introducen oraciones coordinadas y subordinadas</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Ordena oraciones compuestas según nexos</t>
-  </si>
-  <si>
-    <t>Actividad para trabajar las oraciones compuestas mediante nexos</t>
-  </si>
-  <si>
     <t xml:space="preserve">El paréntesis </t>
   </si>
   <si>
-    <t>Actividad para prestar atención a los signos de puntuación de un fragmento teatral, especialmente por lo que respecta al guion y los paréntesis</t>
-  </si>
-  <si>
     <t>Debe incluirse 10 preguntas abiertas:3 sobre literatura; 2 sobre oración compuesta, 3 sobre ortografía (raya, guion, paréntesis) 2 sobre el ensayo. Debe marcarse en el greco Gestor de actividades como actividad didáctica.</t>
   </si>
   <si>
-    <t>Literatura: el Realismo mágico</t>
-  </si>
-  <si>
-    <t>Actividad para construir oraciones compuestas</t>
-  </si>
-  <si>
-    <t>Ortografía: ubica paréntesis</t>
-  </si>
-  <si>
     <t>Cuatro años a bordo de mí mismo</t>
   </si>
   <si>
-    <t xml:space="preserve">El sello literario de Márquez </t>
-  </si>
-  <si>
-    <t>Determina las características literarias</t>
-  </si>
-  <si>
-    <t>Actividad para identificar el enfoque literario de Márquez</t>
-  </si>
-  <si>
-    <t>Interactivo para distinguir el desarrollo literario</t>
-  </si>
-  <si>
-    <t>Analiza la obra</t>
+    <t>Refuerza tu aprendizaje: La novela colombiana del siglo XX</t>
+  </si>
+  <si>
+    <t>Seleccionar 6 frases de textos literarios o periodísticos en donde sea necesario el uso del paréntesis para que los estudiantes los relacionen a nivel de significado y contexto.</t>
+  </si>
+  <si>
+    <t>Actividad para comprender la intencionalidad de los ensayos</t>
+  </si>
+  <si>
+    <t>6 preguntas que guíen al estudiante a identificar la intencionalidad de los ensayos.</t>
+  </si>
+  <si>
+    <t>Actividad para identificar las hipótesis de los ensayos</t>
+  </si>
+  <si>
+    <t>6 imágenes acompañadas de preguntas que permitan inferir títulos de ensayos.</t>
+  </si>
+  <si>
+    <t>8 preguntas relacionadas con el desarrollo de la novela del siglo XX a partir de los autores vistos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 o 6 parejas de oraciones compuestas. </t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La oración compuesta</t>
+  </si>
+  <si>
+    <t>Actividad para analizar oraciones compuestas</t>
+  </si>
+  <si>
+    <t>Determina la intención comunicativa</t>
+  </si>
+  <si>
+    <t>Cómo leer un ensayo</t>
+  </si>
+  <si>
+    <t>Interactivo que expone estrategias para analizar un ensayo</t>
+  </si>
+  <si>
+    <t>8 preguntas relacionadas con los elementos, la estructura y las claves de un ensayo.</t>
+  </si>
+  <si>
+    <t>Interactivo para planear la escritura de un ensayo</t>
+  </si>
+  <si>
+    <t>Actividad para distinguir las pautas para escribir un ensayo</t>
+  </si>
+  <si>
+    <t>Actividad para determinar el desarrollo de la novela en Colombia</t>
+  </si>
+  <si>
+    <t>Gramática: clasifica las  oraciones compuestas</t>
+  </si>
+  <si>
+    <t>Se invita a los estudiantes a ordenar una secuencia de sugerencias para organizar y redactar un ensayo.</t>
+  </si>
+  <si>
+    <t>Exposición e oraciones y preguntas que guíen al análisis sintáctico de las oraciones compuestas.</t>
+  </si>
+  <si>
+    <t>Un fragmento literario para que los estudiantes seleccionen de la lista desplegable la raya o el guion según corresponda.</t>
+  </si>
+  <si>
+    <t>Fragmentos literarios, periodísticos, científicos que tengan el uso de paréntesis para que los estudiantes por medio de preguntas infieran su uso.</t>
+  </si>
+  <si>
+    <t>Actividad para identificar el enfoque comunicativo del ensayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fragmento relacionado con la intencionalidad comunicativa de un ensayo, para que los estudiantes lo completen con palabras claves que argumenten su propósito. </t>
+  </si>
+  <si>
+    <t>Actividad para determinar las características de un ensayo</t>
+  </si>
+  <si>
+    <t>Secuencia de características por orden de importancia de un ensayo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expone claves técnicas o metodologías de lectura para comprender, inferir e interpretar un ensayo. </t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Características de un ensayo</t>
+  </si>
+  <si>
+    <t>8 preguntas de interpretación en inferencia que guíen al estudiante en la producción de un ensayo.</t>
+  </si>
+  <si>
+    <t>Subsistema (sección 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para identificar el uso de los signos de puntuación </t>
+  </si>
+  <si>
+    <t>Preguntas relacionadas con el contexto, los personajes, el género y el estilo de la obra.</t>
+  </si>
+  <si>
+    <t>Contenedores de oraciones compuestas copulativas, adversativas, disyuntivas y distributivas para que los estudiantes las ubiquen en el lugar que correspondan.</t>
+  </si>
+  <si>
+    <t>Preguntas relacionadas con el desarrollo de la novela en Colombia en el siglo XX.</t>
+  </si>
+  <si>
+    <t>Párrafo que contenga los elementos clave de un ensayo.</t>
+  </si>
+  <si>
+    <t>6 dictados de fragmentos de diferentes géneros literarios con uso de la raya, el guion y el paréntesis.</t>
+  </si>
+  <si>
+    <t>Fragmentos literarios claves del desarrollo de las partes de la obra.</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>Recursos M</t>
+  </si>
+  <si>
+    <t>Recurso M5D-01</t>
+  </si>
+  <si>
+    <t>RM_01_01_CO</t>
+  </si>
+  <si>
+    <t>Recurso M2A-01</t>
+  </si>
+  <si>
+    <t>Recurso M6B-01</t>
+  </si>
+  <si>
+    <t>Recurso M1C-01</t>
+  </si>
+  <si>
+    <t>Recurso M101A-01</t>
+  </si>
+  <si>
+    <t>Recurso M101A-02</t>
+  </si>
+  <si>
+    <t>Recurso M101A-03</t>
+  </si>
+  <si>
+    <t>Recurso M101A-04</t>
+  </si>
+  <si>
+    <t>Recurso M101A-05</t>
+  </si>
+  <si>
+    <t>Recurso M5A-01</t>
+  </si>
+  <si>
+    <t>Recurso M5A-02</t>
+  </si>
+  <si>
+    <t>Recurso M5D-02</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>Recursos F</t>
+  </si>
+  <si>
+    <t>Recurso F7-01</t>
+  </si>
+  <si>
+    <t>RF_01_01_CO</t>
+  </si>
+  <si>
+    <t>Recurso M4A-01</t>
+  </si>
+  <si>
+    <t>Recurso M4A-02</t>
+  </si>
+  <si>
+    <t>Recurso M12A-01</t>
+  </si>
+  <si>
+    <t>Recurso M12A-02</t>
+  </si>
+  <si>
+    <t>Recurso M12A-03</t>
+  </si>
+  <si>
+    <t>Recurso M6A-01</t>
+  </si>
+  <si>
+    <t>Recurso F6B-01</t>
+  </si>
+  <si>
+    <t>Recurso M2C-01</t>
+  </si>
+  <si>
+    <t>Recurso M2A-02</t>
+  </si>
+  <si>
+    <t>Recurso M2A-03</t>
+  </si>
+  <si>
+    <t>Recurso M10A-01</t>
+  </si>
+  <si>
+    <t>Recurso M101AP-01</t>
+  </si>
+  <si>
+    <t>Recurso F10-01</t>
+  </si>
+  <si>
+    <t>Recurso F13B-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccionar un fragmento de la obra de Gabriel García Márquez y a partir de él realizar 5 preguntas que determinen las características literarias del autor. </t>
+  </si>
+  <si>
+    <t>Fragmentos de diferentes obras de Gabriel García Márquez con preguntas que guíen al estudiante a determinar las características y el enfoque literario, histórico y cultural . DBA:Relaciona los significados de los textos que lee con los contextos sociales, culturales, políticos y económicos en que se han producido.</t>
+  </si>
+  <si>
+    <t>Interactivo que expone datos biográficos, criticas literarias, una especie de línea de tiempo de las obras de Márquez y mención de Premio Nobel. DBA:Relaciona los significados de los textos que lee con los contextos sociales, culturales, políticos y económicos en que se han producido.</t>
+  </si>
+  <si>
+    <t>Revisar el recurso y ajustar el vocabulario y el lenguaje a nuestro contexto. Si considera pertinente ampliarlo lo puede hacer. DBA: Aplica todas las etapas de la escritura en la elaboración de textos coherentes y cohesionados, con criterios cercanos a los de una publicación.</t>
+  </si>
+  <si>
+    <t>Seguir instrucciones del documento de Word para el desarrollo del motor. DBA: Consulta, sintetiza y evalúa la información extraída de diferentes fuentes para realizar un trabajo académico. DBA: Desarrolla un tema de un área disciplinar, teniendo en cuenta: los hechos relevantes, detalles concretos, citas, referencias y vocabulario específico.</t>
+  </si>
+  <si>
+    <t>Seleccionar fragmentos literarios de los autores vistos de las mismas y de otras obras para enfatizar en los estilos literarios y en su influencia literaria. De ser posible retomar fragmentos de críticos literarios. DBA: Hace un juicio valorativo de un aspecto característico como el tiempo, el lugar o los personajes de un texto literario.           DBA: Aprecia el legado literario colombiano y latinoamericano,
+mediante la lectura de textos de ficción y no ficción, poesía, ensayos y obras periodísticas.</t>
+  </si>
+  <si>
+    <t>Preguntas de análisis e interpretación de los contextos que trata la obra citada, como la música, la ciudad, las drogas, entre otros temas. DBA: Identifica el contexto social, histórico, político y cultural de las obras, para ampliar el análisis y la evaluación del texto.</t>
+  </si>
+  <si>
+    <t>Recurso M5B-01</t>
+  </si>
+  <si>
+    <t>Seleccionar un VIDEO  de Aula planeta y a partir de él crear 6 o 7 preguntas para que los estudiantes seleccionen respuestas que contienen oraciones con sujeto y predicado o solo sujetos o solo predicados o mezclados. Sugiero el video titulado Fisetas de San Juan en Ciudadela http://hispanicasaber.planetasaber.com/encyclopedia/default.asp?idpack=10&amp;idpil=VI002097&amp;ruta=Mediateca</t>
+  </si>
+  <si>
+    <t>Recurso M5D-03</t>
+  </si>
+  <si>
+    <t>Recurso M1C-02</t>
+  </si>
+  <si>
+    <t>Literatura: caracteriza el Realismo mágico</t>
+  </si>
+  <si>
+    <t>Gramática: identifica enlaces gramaticales</t>
+  </si>
+  <si>
+    <t>Ortografía: reconoce los signos de puntuación</t>
+  </si>
+  <si>
+    <t>Ortografía: relaciona enunciados</t>
+  </si>
+  <si>
+    <t>Comprensión textual: el propósito de un ensayo</t>
+  </si>
+  <si>
+    <t>Producción textual: identifica títulos de ensayos</t>
+  </si>
+  <si>
+    <t>Reconoce temas literarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sello literario de García Márquez </t>
+  </si>
+  <si>
+    <t>Comprende  la obra Cien años de soledad</t>
+  </si>
+  <si>
+    <t>Determina la secuencia literaria</t>
+  </si>
+  <si>
+    <t>Infiere ideas</t>
+  </si>
+  <si>
+    <t>Reconoce predicados</t>
+  </si>
+  <si>
+    <t>Relaciona oraciones compuestas</t>
+  </si>
+  <si>
+    <t>Clasifica los nexos</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Caracteriza las oraciones compuestas</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Ordena oraciones compuestas según el nexo</t>
+  </si>
+  <si>
+    <t>Selecciona el signo ortográfico</t>
+  </si>
+  <si>
+    <t>Analiza  el uso del paréntesis</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Uso del paréntesis, del guion y de la raya</t>
+  </si>
+  <si>
+    <t>Caracteriza un ensayo</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Comprende un ensayo</t>
+  </si>
+  <si>
+    <t>Literatura: la novela colombiana</t>
+  </si>
+  <si>
+    <t>Ortografía: define los signos de ortográficos</t>
+  </si>
+  <si>
+    <t>Comprensión textual: caracteriza un ensayo</t>
+  </si>
+  <si>
+    <t>Producción textual: ordena los pasos de un ensayo</t>
+  </si>
+  <si>
+    <t>Banco de actividades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para identificar el estilo literario de Gabriel García Márquez </t>
+  </si>
+  <si>
+    <t>Actividad para completar oraciones compuestas a partir de enlaces gramaticales</t>
+  </si>
+  <si>
+    <t>Actividad para determinar el uso del paréntesis de acuerdo al contexto</t>
+  </si>
+  <si>
+    <t>Actividad para identificar las temáticas de algunas obras de Gabriel García Márquez</t>
+  </si>
+  <si>
+    <t>Interactivo para distinguir el desarrollo literario de García Márquez</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Actividad para interpretar </t>
+      <t xml:space="preserve">Actividad para inferir ideas explicitas e implicitas en la obra </t>
     </r>
     <r>
       <rPr>
@@ -711,314 +967,80 @@
     </r>
   </si>
   <si>
-    <t>Secuencia literaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad para determinar las etapas de la obra </t>
-  </si>
-  <si>
-    <t>Relaciona contextos</t>
-  </si>
-  <si>
-    <t>Actividad para identificar los temas de la obra</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: La novela colombiana del siglo XX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad para determinar el uso del paréntesis </t>
-  </si>
-  <si>
-    <t>Seleccionar 6 frases de textos literarios o periodísticos en donde sea necesario el uso del paréntesis para que los estudiantes los relacionen a nivel de significado y contexto.</t>
-  </si>
-  <si>
-    <t>Actividad para comprender la intencionalidad de los ensayos</t>
-  </si>
-  <si>
-    <t>6 preguntas que guíen al estudiante a identificar la intencionalidad de los ensayos.</t>
-  </si>
-  <si>
-    <t>Actividad para identificar las hipótesis de los ensayos</t>
-  </si>
-  <si>
-    <t>6 imágenes acompañadas de preguntas que permitan inferir títulos de ensayos.</t>
-  </si>
-  <si>
-    <t>Actividad que distingue las características literarias de la novela</t>
-  </si>
-  <si>
-    <t>8 preguntas relacionadas con el desarrollo de la novela del siglo XX a partir de los autores vistos.</t>
-  </si>
-  <si>
-    <t>Interactivo que expone fragmentos literarios d ella novela colombiana.</t>
-  </si>
-  <si>
-    <t>Ordena secuencia  de predicados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad para determinar el uso de predicados </t>
-  </si>
-  <si>
-    <t>Relaciona proposiciones</t>
-  </si>
-  <si>
-    <t>Actividad para asociar proposiciones de oraciones compuestas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 o 6 parejas de oraciones compuestas. </t>
-  </si>
-  <si>
-    <t>Distingue el uso de la raya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad para diferenciar el uso de la raya de acuerdo a los contextos </t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: La oración compuesta</t>
-  </si>
-  <si>
-    <t>Actividad para analizar oraciones compuestas</t>
-  </si>
-  <si>
-    <t>Determina la intención comunicativa</t>
-  </si>
-  <si>
-    <t>Cómo leer un ensayo</t>
-  </si>
-  <si>
-    <t>Interactivo que expone estrategias para analizar un ensayo</t>
-  </si>
-  <si>
-    <t>Reconoce un ensayo</t>
-  </si>
-  <si>
-    <t>Actividad para determinar los elementos de un ensayo</t>
-  </si>
-  <si>
-    <t>8 preguntas relacionadas con los elementos, la estructura y las claves de un ensayo.</t>
-  </si>
-  <si>
-    <t>Interactivo para planear la escritura de un ensayo</t>
-  </si>
-  <si>
-    <t>Actividad para distinguir las pautas para escribir un ensayo</t>
-  </si>
-  <si>
-    <t>Literatura: La novela colombiana</t>
-  </si>
-  <si>
-    <t>Actividad para determinar el desarrollo de la novela en Colombia</t>
-  </si>
-  <si>
-    <t>Actividad para reconocer las partes de un ensayo</t>
-  </si>
-  <si>
-    <t>Gramática: clasifica las  oraciones compuestas</t>
-  </si>
-  <si>
-    <t>Actividad para distinguir las oraciones compuestas</t>
-  </si>
-  <si>
-    <t>Actividad para reconocer la estructura de un ensayo</t>
-  </si>
-  <si>
-    <t>Se invita a los estudiantes a ordenar una secuencia de sugerencias para organizar y redactar un ensayo.</t>
-  </si>
-  <si>
-    <t>Producción textual: determina títulos de ensayos</t>
-  </si>
-  <si>
-    <t>Exposición e oraciones y preguntas que guíen al análisis sintáctico de las oraciones compuestas.</t>
-  </si>
-  <si>
-    <t>Un fragmento literario para que los estudiantes seleccionen de la lista desplegable la raya o el guion según corresponda.</t>
-  </si>
-  <si>
-    <t>Comprende el uso de paréntesis</t>
-  </si>
-  <si>
-    <t>Actividad para distinguir el significado del uso del paréntesis</t>
-  </si>
-  <si>
-    <t>Fragmentos literarios, periodísticos, científicos que tengan el uso de paréntesis para que los estudiantes por medio de preguntas infieran su uso.</t>
-  </si>
-  <si>
-    <t>Actividad para identificar el enfoque comunicativo del ensayo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fragmento relacionado con la intencionalidad comunicativa de un ensayo, para que los estudiantes lo completen con palabras claves que argumenten su propósito. </t>
-  </si>
-  <si>
-    <t>Actividad para determinar las características de un ensayo</t>
-  </si>
-  <si>
-    <t>Secuencia de características por orden de importancia de un ensayo.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expone claves técnicas o metodologías de lectura para comprender, inferir e interpretar un ensayo. </t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Características de un ensayo</t>
-  </si>
-  <si>
-    <t>8 preguntas de interpretación en inferencia que guíen al estudiante en la producción de un ensayo.</t>
-  </si>
-  <si>
-    <t>Subsistema (sección 3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad para identificar el uso de los signos de puntuación </t>
-  </si>
-  <si>
-    <t>Preguntas relacionadas con el contexto, los personajes, el género y el estilo de la obra.</t>
-  </si>
-  <si>
-    <t>Contenedores de oraciones compuestas copulativas, adversativas, disyuntivas y distributivas para que los estudiantes las ubiquen en el lugar que correspondan.</t>
-  </si>
-  <si>
-    <t>Preguntas relacionadas con el desarrollo de la novela en Colombia en el siglo XX.</t>
-  </si>
-  <si>
-    <t>Párrafo que contenga los elementos clave de un ensayo.</t>
-  </si>
-  <si>
-    <t>6 dictados de fragmentos de diferentes géneros literarios con uso de la raya, el guion y el paréntesis.</t>
-  </si>
-  <si>
-    <t>Fragmentos literarios claves del desarrollo de las partes de la obra.</t>
-  </si>
-  <si>
-    <t>RM</t>
-  </si>
-  <si>
-    <t>Recursos M</t>
-  </si>
-  <si>
-    <t>Recurso M5D-01</t>
-  </si>
-  <si>
-    <t>RM_01_01_CO</t>
-  </si>
-  <si>
-    <t>Recurso M2A-01</t>
-  </si>
-  <si>
-    <t>Recurso M6B-01</t>
-  </si>
-  <si>
-    <t>Recurso M1C-01</t>
-  </si>
-  <si>
-    <t>Recurso M101A-01</t>
-  </si>
-  <si>
-    <t>Recurso M101A-02</t>
-  </si>
-  <si>
-    <t>Recurso M101A-03</t>
-  </si>
-  <si>
-    <t>Recurso M101A-04</t>
-  </si>
-  <si>
-    <t>Recurso M101A-05</t>
-  </si>
-  <si>
-    <t>Recurso M5A-01</t>
-  </si>
-  <si>
-    <t>Recurso M5A-02</t>
-  </si>
-  <si>
-    <t>Recurso M5D-02</t>
-  </si>
-  <si>
-    <t>RF</t>
-  </si>
-  <si>
-    <t>Recursos F</t>
-  </si>
-  <si>
-    <t>Recurso F7-01</t>
-  </si>
-  <si>
-    <t>RF_01_01_CO</t>
-  </si>
-  <si>
-    <t>Recurso M4A-01</t>
-  </si>
-  <si>
-    <t>Recurso M4A-02</t>
-  </si>
-  <si>
-    <t>Recurso M12A-01</t>
-  </si>
-  <si>
-    <t>Recurso M12A-02</t>
-  </si>
-  <si>
-    <t>Recurso M12A-03</t>
-  </si>
-  <si>
-    <t>Recurso M6A-01</t>
-  </si>
-  <si>
-    <t>Recurso F6B-01</t>
-  </si>
-  <si>
-    <t>Recurso M2C-01</t>
-  </si>
-  <si>
-    <t>Recurso M2A-02</t>
-  </si>
-  <si>
-    <t>Recurso M2A-03</t>
-  </si>
-  <si>
-    <t>Recurso M10A-01</t>
-  </si>
-  <si>
-    <t>Recurso M101AP-01</t>
-  </si>
-  <si>
-    <t>Recurso F10-01</t>
-  </si>
-  <si>
-    <t>Recurso F13B-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seleccionar un fragmento de la obra de Gabriel García Márquez y a partir de él realizar 5 preguntas que determinen las características literarias del autor. </t>
-  </si>
-  <si>
-    <t>Fragmentos de diferentes obras de Gabriel García Márquez con preguntas que guíen al estudiante a determinar las características y el enfoque literario, histórico y cultural . DBA:Relaciona los significados de los textos que lee con los contextos sociales, culturales, políticos y económicos en que se han producido.</t>
-  </si>
-  <si>
-    <t>Interactivo que expone datos biográficos, criticas literarias, una especie de línea de tiempo de las obras de Márquez y mención de Premio Nobel. DBA:Relaciona los significados de los textos que lee con los contextos sociales, culturales, políticos y económicos en que se han producido.</t>
-  </si>
-  <si>
-    <t>Revisar el recurso y ajustar el vocabulario y el lenguaje a nuestro contexto. Si considera pertinente ampliarlo lo puede hacer. DBA: Aplica todas las etapas de la escritura en la elaboración de textos coherentes y cohesionados, con criterios cercanos a los de una publicación.</t>
-  </si>
-  <si>
-    <t>Seguir instrucciones del documento de Word para el desarrollo del motor. DBA: Consulta, sintetiza y evalúa la información extraída de diferentes fuentes para realizar un trabajo académico. DBA: Desarrolla un tema de un área disciplinar, teniendo en cuenta: los hechos relevantes, detalles concretos, citas, referencias y vocabulario específico.</t>
-  </si>
-  <si>
-    <t>Seleccionar fragmentos literarios de los autores vistos de las mismas y de otras obras para enfatizar en los estilos literarios y en su influencia literaria. De ser posible retomar fragmentos de críticos literarios. DBA: Hace un juicio valorativo de un aspecto característico como el tiempo, el lugar o los personajes de un texto literario.           DBA: Aprecia el legado literario colombiano y latinoamericano,
-mediante la lectura de textos de ficción y no ficción, poesía, ensayos y obras periodísticas.</t>
-  </si>
-  <si>
-    <t>Preguntas de análisis e interpretación de los contextos que trata la obra citada, como la música, la ciudad, las drogas, entre otros temas. DBA: Identifica el contexto social, histórico, político y cultural de las obras, para ampliar el análisis y la evaluación del texto.</t>
-  </si>
-  <si>
-    <t>Recurso M5B-01</t>
-  </si>
-  <si>
-    <t>Seleccionar un VIDEO  de Aula planeta y a partir de él crear 6 o 7 preguntas para que los estudiantes seleccionen respuestas que contienen oraciones con sujeto y predicado o solo sujetos o solo predicados o mezclados. Sugiero el video titulado Fisetas de San Juan en Ciudadela http://hispanicasaber.planetasaber.com/encyclopedia/default.asp?idpack=10&amp;idpil=VI002097&amp;ruta=Mediateca</t>
-  </si>
-  <si>
-    <t>Recurso M5D-03</t>
-  </si>
-  <si>
-    <t>Recurso M1C-02</t>
+    <r>
+      <t xml:space="preserve">Actividad para ordenar las acciones de la obra </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>El amor en los tiempos del cólera</t>
+    </r>
+  </si>
+  <si>
+    <t>Actividad para deducir ideas de la obra  ¡Que viva la música!</t>
+  </si>
+  <si>
+    <t>Actividad para distinguir las características literarias de la novela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo que expone fragmentos de la novela colombiana </t>
+  </si>
+  <si>
+    <t>Actividad para determinar el uso de predicados de acuerdo al contexto</t>
+  </si>
+  <si>
+    <t>Interactivo que expone los pasos para analizar oraciones compuestas</t>
+  </si>
+  <si>
+    <t>Actividad para asociar oraciones compuestas a partir de los nexos</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer los nexos de las oraciones compuestas</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer el tipo  de oración compuesta</t>
+  </si>
+  <si>
+    <t>Actividad para organizar las oraciones compuestas a partir de nexos y signos ortográficos</t>
+  </si>
+  <si>
+    <t>Interactivo que expone el uso de los signos ortográficos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para diferenciar el uso de la raya de otros signos </t>
+  </si>
+  <si>
+    <t>Actividad para distinguir el uso del paréntesis de acuerdo al contexto</t>
+  </si>
+  <si>
+    <t>Actividad para practicar el uso correcto de los signos ortográficos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad para comprender la secuencia narrativa a partir de los signos de puntuación </t>
+  </si>
+  <si>
+    <t>Actividad para inferir ideas explícitas e implícitas en un ensayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo que explica las partes de un ensayo </t>
+  </si>
+  <si>
+    <t>Actividad para distinguir las oraciones compuestas a partir del nexo</t>
+  </si>
+  <si>
+    <t>Actividad para identificar la definición del guion, la raya y el paréntesis</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer las características de un ensayo</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer las pautas para elaborar un ensayo</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1158,6 +1180,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -1214,7 +1242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1285,30 +1313,17 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1386,6 +1401,30 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1693,9 +1732,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P3" sqref="P3:P44"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P44" sqref="P44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1705,17 +1744,17 @@
     <col min="3" max="3" width="13.42578125" style="24" customWidth="1"/>
     <col min="4" max="4" width="35.85546875" style="17" customWidth="1"/>
     <col min="5" max="5" width="36.28515625" style="24" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="39" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="32" customWidth="1"/>
     <col min="7" max="7" width="41.7109375" style="24" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" style="18" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="39" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" style="32" customWidth="1"/>
     <col min="10" max="10" width="41.85546875" style="24" customWidth="1"/>
     <col min="11" max="11" width="16.140625" style="24" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" style="24" customWidth="1"/>
     <col min="13" max="14" width="9.28515625" style="24" customWidth="1"/>
-    <col min="15" max="15" width="39.28515625" style="39" customWidth="1"/>
+    <col min="15" max="15" width="39.28515625" style="32" customWidth="1"/>
     <col min="16" max="16" width="16.5703125" style="18" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="39" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="32" customWidth="1"/>
     <col min="18" max="18" width="23" style="24" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" style="24" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="25.85546875" style="24" bestFit="1" customWidth="1"/>
@@ -1724,96 +1763,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="G1" s="51" t="s">
+      <c r="F1" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="G1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="57"/>
-      <c r="O1" s="45" t="s">
+      <c r="N1" s="50"/>
+      <c r="O1" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="P1" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="60" t="s">
+      <c r="Q1" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="64" t="s">
+      <c r="R1" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="60" t="s">
+      <c r="S1" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="62" t="s">
+      <c r="T1" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="60" t="s">
+      <c r="U1" s="53" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="52"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="45"/>
       <c r="M2" s="25" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="61"/>
-    </row>
-    <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="54"/>
+    </row>
+    <row r="3" spans="1:21" ht="32.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
@@ -1828,8 +1867,8 @@
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="26" t="s">
-        <v>214</v>
+      <c r="G3" s="61" t="s">
+        <v>277</v>
       </c>
       <c r="H3" s="22">
         <v>1</v>
@@ -1837,8 +1876,8 @@
       <c r="I3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="27" t="s">
-        <v>205</v>
+      <c r="J3" s="65" t="s">
+        <v>303</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>20</v>
@@ -1850,8 +1889,8 @@
       <c r="N3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="28" t="s">
-        <v>316</v>
+      <c r="O3" s="26" t="s">
+        <v>266</v>
       </c>
       <c r="P3" s="15" t="s">
         <v>19</v>
@@ -1860,19 +1899,19 @@
         <v>6</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S3" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T3" s="29" t="s">
-        <v>285</v>
+        <v>234</v>
+      </c>
+      <c r="T3" s="27" t="s">
+        <v>235</v>
       </c>
       <c r="U3" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>16</v>
       </c>
@@ -1885,10 +1924,10 @@
       <c r="D4" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="26" t="s">
-        <v>139</v>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="61" t="s">
+        <v>278</v>
       </c>
       <c r="H4" s="16">
         <v>2</v>
@@ -1896,8 +1935,8 @@
       <c r="I4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="32" t="s">
-        <v>215</v>
+      <c r="J4" s="59" t="s">
+        <v>304</v>
       </c>
       <c r="K4" s="12" t="s">
         <v>20</v>
@@ -1909,8 +1948,8 @@
       <c r="N4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="31" t="s">
-        <v>206</v>
+      <c r="O4" s="29" t="s">
+        <v>192</v>
       </c>
       <c r="P4" s="15" t="s">
         <v>19</v>
@@ -1919,19 +1958,19 @@
         <v>6</v>
       </c>
       <c r="R4" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S4" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T4" s="29" t="s">
-        <v>287</v>
+        <v>234</v>
+      </c>
+      <c r="T4" s="27" t="s">
+        <v>237</v>
       </c>
       <c r="U4" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
@@ -1944,10 +1983,10 @@
       <c r="D5" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="26" t="s">
-        <v>207</v>
+      <c r="E5" s="28"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="61" t="s">
+        <v>279</v>
       </c>
       <c r="H5" s="16">
         <v>3</v>
@@ -1955,8 +1994,8 @@
       <c r="I5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="32" t="s">
-        <v>276</v>
+      <c r="J5" s="59" t="s">
+        <v>226</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>20</v>
@@ -1968,8 +2007,8 @@
       <c r="N5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O5" s="31" t="s">
-        <v>281</v>
+      <c r="O5" s="29" t="s">
+        <v>231</v>
       </c>
       <c r="P5" s="15" t="s">
         <v>19</v>
@@ -1978,19 +2017,19 @@
         <v>6</v>
       </c>
       <c r="R5" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S5" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T5" s="29" t="s">
-        <v>288</v>
+        <v>234</v>
+      </c>
+      <c r="T5" s="27" t="s">
+        <v>238</v>
       </c>
       <c r="U5" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>16</v>
       </c>
@@ -2003,10 +2042,10 @@
       <c r="D6" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="26" t="s">
-        <v>216</v>
+      <c r="E6" s="28"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="61" t="s">
+        <v>280</v>
       </c>
       <c r="H6" s="22">
         <v>4</v>
@@ -2014,8 +2053,8 @@
       <c r="I6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="32" t="s">
-        <v>229</v>
+      <c r="J6" s="59" t="s">
+        <v>305</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>20</v>
@@ -2027,8 +2066,8 @@
       <c r="N6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="31" t="s">
-        <v>230</v>
+      <c r="O6" s="29" t="s">
+        <v>197</v>
       </c>
       <c r="P6" s="15" t="s">
         <v>19</v>
@@ -2037,19 +2076,19 @@
         <v>6</v>
       </c>
       <c r="R6" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S6" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T6" s="29" t="s">
-        <v>289</v>
+        <v>234</v>
+      </c>
+      <c r="T6" s="27" t="s">
+        <v>239</v>
       </c>
       <c r="U6" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
@@ -2062,10 +2101,10 @@
       <c r="D7" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="26" t="s">
-        <v>145</v>
+      <c r="E7" s="28"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="61" t="s">
+        <v>281</v>
       </c>
       <c r="H7" s="16">
         <v>5</v>
@@ -2073,8 +2112,8 @@
       <c r="I7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="32" t="s">
-        <v>231</v>
+      <c r="J7" s="59" t="s">
+        <v>198</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>20</v>
@@ -2086,8 +2125,8 @@
       <c r="N7" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="31" t="s">
-        <v>232</v>
+      <c r="O7" s="29" t="s">
+        <v>199</v>
       </c>
       <c r="P7" s="15" t="s">
         <v>19</v>
@@ -2096,19 +2135,19 @@
         <v>6</v>
       </c>
       <c r="R7" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S7" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T7" s="29" t="s">
-        <v>290</v>
+        <v>234</v>
+      </c>
+      <c r="T7" s="27" t="s">
+        <v>240</v>
       </c>
       <c r="U7" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
@@ -2121,10 +2160,10 @@
       <c r="D8" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="26" t="s">
-        <v>262</v>
+      <c r="E8" s="28"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="61" t="s">
+        <v>282</v>
       </c>
       <c r="H8" s="16">
         <v>6</v>
@@ -2132,8 +2171,8 @@
       <c r="I8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="32" t="s">
-        <v>233</v>
+      <c r="J8" s="59" t="s">
+        <v>200</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>20</v>
@@ -2145,8 +2184,8 @@
       <c r="N8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="31" t="s">
-        <v>234</v>
+      <c r="O8" s="29" t="s">
+        <v>201</v>
       </c>
       <c r="P8" s="15" t="s">
         <v>19</v>
@@ -2155,19 +2194,19 @@
         <v>6</v>
       </c>
       <c r="R8" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S8" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T8" s="29" t="s">
-        <v>295</v>
+        <v>234</v>
+      </c>
+      <c r="T8" s="27" t="s">
+        <v>245</v>
       </c>
       <c r="U8" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
@@ -2180,12 +2219,12 @@
       <c r="D9" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E9" s="30" t="s">
-        <v>217</v>
-      </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="26" t="s">
-        <v>219</v>
+      <c r="E9" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="29"/>
+      <c r="G9" s="61" t="s">
+        <v>283</v>
       </c>
       <c r="H9" s="22">
         <v>7</v>
@@ -2193,8 +2232,8 @@
       <c r="I9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="32" t="s">
-        <v>220</v>
+      <c r="J9" s="59" t="s">
+        <v>306</v>
       </c>
       <c r="K9" s="12" t="s">
         <v>20</v>
@@ -2206,8 +2245,8 @@
       <c r="N9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="O9" s="31" t="s">
-        <v>317</v>
+      <c r="O9" s="29" t="s">
+        <v>267</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>19</v>
@@ -2216,19 +2255,19 @@
         <v>6</v>
       </c>
       <c r="R9" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S9" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T9" s="29" t="s">
-        <v>297</v>
+        <v>234</v>
+      </c>
+      <c r="T9" s="27" t="s">
+        <v>247</v>
       </c>
       <c r="U9" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -2241,12 +2280,12 @@
       <c r="D10" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="E10" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="26" t="s">
-        <v>218</v>
+      <c r="F10" s="29"/>
+      <c r="G10" s="61" t="s">
+        <v>284</v>
       </c>
       <c r="H10" s="16">
         <v>8</v>
@@ -2254,8 +2293,8 @@
       <c r="I10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="32" t="s">
-        <v>221</v>
+      <c r="J10" s="59" t="s">
+        <v>307</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>20</v>
@@ -2267,8 +2306,8 @@
         <v>56</v>
       </c>
       <c r="N10" s="6"/>
-      <c r="O10" s="31" t="s">
-        <v>318</v>
+      <c r="O10" s="29" t="s">
+        <v>268</v>
       </c>
       <c r="P10" s="15" t="s">
         <v>19</v>
@@ -2277,19 +2316,19 @@
         <v>6</v>
       </c>
       <c r="R10" s="20" t="s">
-        <v>298</v>
+        <v>248</v>
       </c>
       <c r="S10" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="T10" s="29" t="s">
-        <v>300</v>
+        <v>249</v>
+      </c>
+      <c r="T10" s="27" t="s">
+        <v>250</v>
       </c>
       <c r="U10" s="19" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
@@ -2302,12 +2341,12 @@
       <c r="D11" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="26" t="s">
-        <v>222</v>
+      <c r="F11" s="29"/>
+      <c r="G11" s="61" t="s">
+        <v>285</v>
       </c>
       <c r="H11" s="16">
         <v>9</v>
@@ -2315,8 +2354,8 @@
       <c r="I11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="32" t="s">
-        <v>223</v>
+      <c r="J11" s="59" t="s">
+        <v>308</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>20</v>
@@ -2328,8 +2367,8 @@
       <c r="N11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O11" s="33" t="s">
-        <v>277</v>
+      <c r="O11" s="30" t="s">
+        <v>227</v>
       </c>
       <c r="P11" s="15" t="s">
         <v>19</v>
@@ -2338,19 +2377,19 @@
         <v>6</v>
       </c>
       <c r="R11" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S11" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T11" s="29" t="s">
-        <v>302</v>
+        <v>234</v>
+      </c>
+      <c r="T11" s="27" t="s">
+        <v>252</v>
       </c>
       <c r="U11" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
@@ -2363,12 +2402,12 @@
       <c r="D12" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="G12" s="26" t="s">
-        <v>224</v>
+      <c r="F12" s="29"/>
+      <c r="G12" s="61" t="s">
+        <v>286</v>
       </c>
       <c r="H12" s="22">
         <v>10</v>
@@ -2376,8 +2415,8 @@
       <c r="I12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="32" t="s">
-        <v>225</v>
+      <c r="J12" s="59" t="s">
+        <v>309</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>20</v>
@@ -2389,29 +2428,29 @@
       <c r="N12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="O12" s="31" t="s">
-        <v>282</v>
-      </c>
-      <c r="P12" s="16" t="s">
+      <c r="O12" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="P12" s="66" t="s">
         <v>20</v>
       </c>
       <c r="Q12" s="19">
         <v>6</v>
       </c>
       <c r="R12" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S12" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T12" s="29" t="s">
-        <v>304</v>
+        <v>234</v>
+      </c>
+      <c r="T12" s="27" t="s">
+        <v>254</v>
       </c>
       <c r="U12" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -2424,12 +2463,12 @@
       <c r="D13" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="26" t="s">
-        <v>226</v>
+      <c r="F13" s="29"/>
+      <c r="G13" s="61" t="s">
+        <v>287</v>
       </c>
       <c r="H13" s="16">
         <v>11</v>
@@ -2437,8 +2476,8 @@
       <c r="I13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="32" t="s">
-        <v>227</v>
+      <c r="J13" s="59" t="s">
+        <v>310</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>20</v>
@@ -2450,8 +2489,8 @@
       <c r="N13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="O13" s="31" t="s">
-        <v>322</v>
+      <c r="O13" s="29" t="s">
+        <v>272</v>
       </c>
       <c r="P13" s="15" t="s">
         <v>19</v>
@@ -2460,19 +2499,19 @@
         <v>6</v>
       </c>
       <c r="R13" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S13" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T13" s="29" t="s">
-        <v>307</v>
+        <v>234</v>
+      </c>
+      <c r="T13" s="27" t="s">
+        <v>257</v>
       </c>
       <c r="U13" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
@@ -2485,12 +2524,12 @@
       <c r="D14" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="F14" s="31"/>
-      <c r="G14" s="26" t="s">
-        <v>228</v>
+      <c r="F14" s="29"/>
+      <c r="G14" s="61" t="s">
+        <v>196</v>
       </c>
       <c r="H14" s="16">
         <v>12</v>
@@ -2498,8 +2537,8 @@
       <c r="I14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="32" t="s">
-        <v>235</v>
+      <c r="J14" s="59" t="s">
+        <v>311</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>20</v>
@@ -2511,8 +2550,8 @@
       <c r="N14" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="O14" s="31" t="s">
-        <v>236</v>
+      <c r="O14" s="29" t="s">
+        <v>202</v>
       </c>
       <c r="P14" s="15" t="s">
         <v>19</v>
@@ -2521,19 +2560,19 @@
         <v>6</v>
       </c>
       <c r="R14" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S14" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T14" s="29" t="s">
-        <v>291</v>
+        <v>234</v>
+      </c>
+      <c r="T14" s="27" t="s">
+        <v>241</v>
       </c>
       <c r="U14" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
@@ -2546,11 +2585,11 @@
       <c r="D15" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="26" t="s">
+      <c r="F15" s="29"/>
+      <c r="G15" s="61" t="s">
         <v>129</v>
       </c>
       <c r="H15" s="22">
@@ -2559,8 +2598,8 @@
       <c r="I15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="32" t="s">
-        <v>237</v>
+      <c r="J15" s="59" t="s">
+        <v>312</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>20</v>
@@ -2572,8 +2611,8 @@
         <v>55</v>
       </c>
       <c r="N15" s="6"/>
-      <c r="O15" s="31" t="s">
-        <v>321</v>
+      <c r="O15" s="29" t="s">
+        <v>271</v>
       </c>
       <c r="P15" s="15" t="s">
         <v>19</v>
@@ -2582,19 +2621,19 @@
         <v>6</v>
       </c>
       <c r="R15" s="20" t="s">
-        <v>298</v>
+        <v>248</v>
       </c>
       <c r="S15" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="T15" s="29" t="s">
-        <v>308</v>
+        <v>249</v>
+      </c>
+      <c r="T15" s="27" t="s">
+        <v>258</v>
       </c>
       <c r="U15" s="19" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
@@ -2607,12 +2646,12 @@
       <c r="D16" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="F16" s="31"/>
-      <c r="G16" s="26" t="s">
-        <v>162</v>
+      <c r="F16" s="29"/>
+      <c r="G16" s="61" t="s">
+        <v>159</v>
       </c>
       <c r="H16" s="16">
         <v>14</v>
@@ -2620,8 +2659,8 @@
       <c r="I16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="32" t="s">
-        <v>163</v>
+      <c r="J16" s="59" t="s">
+        <v>160</v>
       </c>
       <c r="K16" s="5" t="s">
         <v>19</v>
@@ -2631,7 +2670,7 @@
       </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
-      <c r="O16" s="31" t="s">
+      <c r="O16" s="29" t="s">
         <v>128</v>
       </c>
       <c r="P16" s="16" t="s">
@@ -2641,19 +2680,19 @@
         <v>8</v>
       </c>
       <c r="R16" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="S16" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="T16" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="S16" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="T16" s="29" t="s">
-        <v>162</v>
-      </c>
       <c r="U16" s="19" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
@@ -2666,14 +2705,14 @@
       <c r="D17" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="G17" s="26" t="s">
-        <v>238</v>
+      <c r="G17" s="61" t="s">
+        <v>288</v>
       </c>
       <c r="H17" s="16">
         <v>15</v>
@@ -2681,8 +2720,8 @@
       <c r="I17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="32" t="s">
-        <v>239</v>
+      <c r="J17" s="59" t="s">
+        <v>313</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>20</v>
@@ -2694,8 +2733,8 @@
       <c r="N17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="O17" s="31" t="s">
-        <v>324</v>
+      <c r="O17" s="29" t="s">
+        <v>274</v>
       </c>
       <c r="P17" s="16" t="s">
         <v>19</v>
@@ -2704,19 +2743,19 @@
         <v>6</v>
       </c>
       <c r="R17" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S17" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T17" s="29" t="s">
-        <v>323</v>
+        <v>234</v>
+      </c>
+      <c r="T17" s="27" t="s">
+        <v>273</v>
       </c>
       <c r="U17" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
@@ -2729,12 +2768,12 @@
       <c r="D18" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="26" t="s">
-        <v>165</v>
+      <c r="F18" s="29"/>
+      <c r="G18" s="61" t="s">
+        <v>162</v>
       </c>
       <c r="H18" s="22">
         <v>16</v>
@@ -2742,8 +2781,8 @@
       <c r="I18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="32" t="s">
-        <v>167</v>
+      <c r="J18" s="59" t="s">
+        <v>314</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>19</v>
@@ -2753,7 +2792,7 @@
       </c>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
-      <c r="O18" s="31" t="s">
+      <c r="O18" s="29" t="s">
         <v>128</v>
       </c>
       <c r="P18" s="16" t="s">
@@ -2763,19 +2802,19 @@
         <v>10</v>
       </c>
       <c r="R18" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S18" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="T18" s="29" t="s">
-        <v>165</v>
+        <v>161</v>
+      </c>
+      <c r="T18" s="27" t="s">
+        <v>162</v>
       </c>
       <c r="U18" s="19" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
@@ -2788,12 +2827,12 @@
       <c r="D19" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="26" t="s">
-        <v>172</v>
+      <c r="F19" s="29"/>
+      <c r="G19" s="61" t="s">
+        <v>167</v>
       </c>
       <c r="H19" s="16">
         <v>17</v>
@@ -2801,8 +2840,8 @@
       <c r="I19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="32" t="s">
-        <v>173</v>
+      <c r="J19" s="59" t="s">
+        <v>168</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>19</v>
@@ -2812,7 +2851,7 @@
       </c>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
-      <c r="O19" s="31" t="s">
+      <c r="O19" s="29" t="s">
         <v>128</v>
       </c>
       <c r="P19" s="16" t="s">
@@ -2822,19 +2861,19 @@
         <v>9</v>
       </c>
       <c r="R19" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S19" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="T19" s="29" t="s">
-        <v>175</v>
+        <v>169</v>
+      </c>
+      <c r="T19" s="27" t="s">
+        <v>170</v>
       </c>
       <c r="U19" s="19" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>16</v>
       </c>
@@ -2847,14 +2886,14 @@
       <c r="D20" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="G20" s="26" t="s">
-        <v>240</v>
+      <c r="G20" s="61" t="s">
+        <v>289</v>
       </c>
       <c r="H20" s="16">
         <v>18</v>
@@ -2862,8 +2901,8 @@
       <c r="I20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="32" t="s">
-        <v>241</v>
+      <c r="J20" s="59" t="s">
+        <v>315</v>
       </c>
       <c r="K20" s="5" t="s">
         <v>20</v>
@@ -2875,8 +2914,8 @@
       <c r="N20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O20" s="31" t="s">
-        <v>242</v>
+      <c r="O20" s="29" t="s">
+        <v>203</v>
       </c>
       <c r="P20" s="16" t="s">
         <v>19</v>
@@ -2885,19 +2924,19 @@
         <v>6</v>
       </c>
       <c r="R20" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S20" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T20" s="29" t="s">
-        <v>326</v>
+        <v>234</v>
+      </c>
+      <c r="T20" s="27" t="s">
+        <v>276</v>
       </c>
       <c r="U20" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>16</v>
       </c>
@@ -2910,12 +2949,12 @@
       <c r="D21" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="26" t="s">
-        <v>168</v>
+      <c r="F21" s="29"/>
+      <c r="G21" s="61" t="s">
+        <v>290</v>
       </c>
       <c r="H21" s="22">
         <v>19</v>
@@ -2923,8 +2962,8 @@
       <c r="I21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="32" t="s">
-        <v>208</v>
+      <c r="J21" s="59" t="s">
+        <v>316</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>19</v>
@@ -2934,7 +2973,7 @@
       </c>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="31" t="s">
+      <c r="O21" s="29" t="s">
         <v>128</v>
       </c>
       <c r="P21" s="16" t="s">
@@ -2944,19 +2983,19 @@
         <v>10</v>
       </c>
       <c r="R21" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S21" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="T21" s="29" t="s">
-        <v>170</v>
+        <v>164</v>
+      </c>
+      <c r="T21" s="27" t="s">
+        <v>165</v>
       </c>
       <c r="U21" s="19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
@@ -2969,12 +3008,12 @@
       <c r="D22" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="34" t="s">
-        <v>177</v>
+      <c r="F22" s="29"/>
+      <c r="G22" s="62" t="s">
+        <v>291</v>
       </c>
       <c r="H22" s="16">
         <v>20</v>
@@ -2982,8 +3021,8 @@
       <c r="I22" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="35" t="s">
-        <v>181</v>
+      <c r="J22" s="60" t="s">
+        <v>317</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>19</v>
@@ -2993,29 +3032,29 @@
       </c>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="31" t="s">
+      <c r="O22" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="P22" s="16" t="s">
+      <c r="P22" s="66" t="s">
         <v>20</v>
       </c>
       <c r="Q22" s="19">
         <v>9</v>
       </c>
       <c r="R22" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S22" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="T22" s="29" t="s">
-        <v>179</v>
+        <v>172</v>
+      </c>
+      <c r="T22" s="27" t="s">
+        <v>173</v>
       </c>
       <c r="U22" s="19" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>16</v>
       </c>
@@ -3028,12 +3067,12 @@
       <c r="D23" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="F23" s="31"/>
-      <c r="G23" s="34" t="s">
-        <v>209</v>
+      <c r="F23" s="29"/>
+      <c r="G23" s="62" t="s">
+        <v>292</v>
       </c>
       <c r="H23" s="16">
         <v>21</v>
@@ -3041,8 +3080,8 @@
       <c r="I23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="35" t="s">
-        <v>210</v>
+      <c r="J23" s="60" t="s">
+        <v>318</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>19</v>
@@ -3052,29 +3091,29 @@
       </c>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
-      <c r="O23" s="31" t="s">
+      <c r="O23" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="P23" s="16" t="s">
+      <c r="P23" s="66" t="s">
         <v>20</v>
       </c>
       <c r="Q23" s="19">
         <v>9</v>
       </c>
       <c r="R23" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S23" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="T23" s="29" t="s">
-        <v>182</v>
+      <c r="T23" s="27" t="s">
+        <v>175</v>
       </c>
       <c r="U23" s="19" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>16</v>
       </c>
@@ -3087,12 +3126,12 @@
       <c r="D24" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="F24" s="31"/>
-      <c r="G24" s="34" t="s">
-        <v>245</v>
+      <c r="F24" s="29"/>
+      <c r="G24" s="62" t="s">
+        <v>204</v>
       </c>
       <c r="H24" s="22">
         <v>22</v>
@@ -3100,8 +3139,8 @@
       <c r="I24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="35" t="s">
-        <v>246</v>
+      <c r="J24" s="60" t="s">
+        <v>205</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>20</v>
@@ -3113,8 +3152,8 @@
       <c r="N24" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="O24" s="31" t="s">
-        <v>263</v>
+      <c r="O24" s="29" t="s">
+        <v>215</v>
       </c>
       <c r="P24" s="16" t="s">
         <v>19</v>
@@ -3123,19 +3162,19 @@
         <v>6</v>
       </c>
       <c r="R24" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S24" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T24" s="29" t="s">
-        <v>292</v>
+        <v>234</v>
+      </c>
+      <c r="T24" s="27" t="s">
+        <v>242</v>
       </c>
       <c r="U24" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>16</v>
       </c>
@@ -3145,13 +3184,13 @@
       <c r="C25" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="34" t="s">
-        <v>184</v>
+      <c r="E25" s="28"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="62" t="s">
+        <v>177</v>
       </c>
       <c r="H25" s="16">
         <v>23</v>
@@ -3159,8 +3198,8 @@
       <c r="I25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J25" s="32" t="s">
-        <v>185</v>
+      <c r="J25" s="60" t="s">
+        <v>319</v>
       </c>
       <c r="K25" s="5" t="s">
         <v>19</v>
@@ -3170,7 +3209,7 @@
       </c>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
-      <c r="O25" s="31" t="s">
+      <c r="O25" s="29" t="s">
         <v>128</v>
       </c>
       <c r="P25" s="16" t="s">
@@ -3180,19 +3219,19 @@
         <v>10</v>
       </c>
       <c r="R25" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S25" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="T25" s="29" t="s">
-        <v>184</v>
+        <v>178</v>
+      </c>
+      <c r="T25" s="27" t="s">
+        <v>177</v>
       </c>
       <c r="U25" s="19" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>16</v>
       </c>
@@ -3202,15 +3241,15 @@
       <c r="C26" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="F26" s="31"/>
-      <c r="G26" s="26" t="s">
-        <v>243</v>
+      <c r="F26" s="29"/>
+      <c r="G26" s="61" t="s">
+        <v>293</v>
       </c>
       <c r="H26" s="16">
         <v>24</v>
@@ -3218,8 +3257,8 @@
       <c r="I26" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="32" t="s">
-        <v>244</v>
+      <c r="J26" s="59" t="s">
+        <v>320</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>20</v>
@@ -3231,8 +3270,8 @@
       <c r="N26" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O26" s="31" t="s">
-        <v>264</v>
+      <c r="O26" s="29" t="s">
+        <v>216</v>
       </c>
       <c r="P26" s="16" t="s">
         <v>19</v>
@@ -3241,19 +3280,19 @@
         <v>6</v>
       </c>
       <c r="R26" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S26" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T26" s="29" t="s">
-        <v>309</v>
+        <v>234</v>
+      </c>
+      <c r="T26" s="27" t="s">
+        <v>259</v>
       </c>
       <c r="U26" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>16</v>
       </c>
@@ -3263,15 +3302,15 @@
       <c r="C27" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="E27" s="30" t="s">
-        <v>211</v>
-      </c>
-      <c r="F27" s="31"/>
-      <c r="G27" s="26" t="s">
-        <v>265</v>
+      <c r="E27" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="F27" s="29"/>
+      <c r="G27" s="61" t="s">
+        <v>294</v>
       </c>
       <c r="H27" s="22">
         <v>25</v>
@@ -3279,8 +3318,8 @@
       <c r="I27" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="32" t="s">
-        <v>266</v>
+      <c r="J27" s="59" t="s">
+        <v>321</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>20</v>
@@ -3292,8 +3331,8 @@
       <c r="N27" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="O27" s="31" t="s">
-        <v>267</v>
+      <c r="O27" s="29" t="s">
+        <v>217</v>
       </c>
       <c r="P27" s="16" t="s">
         <v>19</v>
@@ -3302,19 +3341,19 @@
         <v>6</v>
       </c>
       <c r="R27" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S27" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T27" s="29" t="s">
-        <v>325</v>
+        <v>234</v>
+      </c>
+      <c r="T27" s="27" t="s">
+        <v>275</v>
       </c>
       <c r="U27" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>16</v>
       </c>
@@ -3324,15 +3363,15 @@
       <c r="C28" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="26" t="s">
-        <v>189</v>
+      <c r="F28" s="29"/>
+      <c r="G28" s="61" t="s">
+        <v>295</v>
       </c>
       <c r="H28" s="16">
         <v>26</v>
@@ -3340,8 +3379,8 @@
       <c r="I28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="32" t="s">
-        <v>190</v>
+      <c r="J28" s="59" t="s">
+        <v>322</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>19</v>
@@ -3351,7 +3390,7 @@
       </c>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
-      <c r="O28" s="31" t="s">
+      <c r="O28" s="29" t="s">
         <v>128</v>
       </c>
       <c r="P28" s="16" t="s">
@@ -3361,19 +3400,19 @@
         <v>10</v>
       </c>
       <c r="R28" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S28" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="T28" s="29" t="s">
-        <v>188</v>
+        <v>178</v>
+      </c>
+      <c r="T28" s="27" t="s">
+        <v>180</v>
       </c>
       <c r="U28" s="19" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>16</v>
       </c>
@@ -3383,15 +3422,15 @@
       <c r="C29" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="E29" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="26" t="s">
-        <v>201</v>
+      <c r="F29" s="29"/>
+      <c r="G29" s="61" t="s">
+        <v>188</v>
       </c>
       <c r="H29" s="16">
         <v>27</v>
@@ -3399,8 +3438,8 @@
       <c r="I29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="32" t="s">
-        <v>212</v>
+      <c r="J29" s="59" t="s">
+        <v>323</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>19</v>
@@ -3410,7 +3449,7 @@
       </c>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
-      <c r="O29" s="31" t="s">
+      <c r="O29" s="29" t="s">
         <v>128</v>
       </c>
       <c r="P29" s="16" t="s">
@@ -3420,19 +3459,19 @@
         <v>8</v>
       </c>
       <c r="R29" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S29" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="T29" s="29" t="s">
-        <v>203</v>
+        <v>189</v>
+      </c>
+      <c r="T29" s="27" t="s">
+        <v>190</v>
       </c>
       <c r="U29" s="19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>16</v>
       </c>
@@ -3445,12 +3484,12 @@
       <c r="D30" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="E30" s="30" t="s">
+      <c r="E30" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="F30" s="31"/>
-      <c r="G30" s="26" t="s">
-        <v>247</v>
+      <c r="F30" s="29"/>
+      <c r="G30" s="61" t="s">
+        <v>206</v>
       </c>
       <c r="H30" s="22">
         <v>28</v>
@@ -3458,8 +3497,8 @@
       <c r="I30" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J30" s="32" t="s">
-        <v>268</v>
+      <c r="J30" s="59" t="s">
+        <v>218</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>20</v>
@@ -3471,8 +3510,8 @@
       <c r="N30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="O30" s="31" t="s">
-        <v>269</v>
+      <c r="O30" s="29" t="s">
+        <v>219</v>
       </c>
       <c r="P30" s="16" t="s">
         <v>19</v>
@@ -3481,19 +3520,19 @@
         <v>6</v>
       </c>
       <c r="R30" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S30" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T30" s="29" t="s">
-        <v>310</v>
+        <v>234</v>
+      </c>
+      <c r="T30" s="27" t="s">
+        <v>260</v>
       </c>
       <c r="U30" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>16</v>
       </c>
@@ -3506,12 +3545,12 @@
       <c r="D31" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="F31" s="31"/>
-      <c r="G31" s="26" t="s">
-        <v>250</v>
+      <c r="F31" s="29"/>
+      <c r="G31" s="61" t="s">
+        <v>296</v>
       </c>
       <c r="H31" s="16">
         <v>29</v>
@@ -3519,8 +3558,8 @@
       <c r="I31" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="32" t="s">
-        <v>270</v>
+      <c r="J31" s="59" t="s">
+        <v>220</v>
       </c>
       <c r="K31" s="5" t="s">
         <v>20</v>
@@ -3532,29 +3571,29 @@
       <c r="N31" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="O31" s="31" t="s">
-        <v>271</v>
+      <c r="O31" s="29" t="s">
+        <v>221</v>
       </c>
       <c r="P31" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q31" s="19">
         <v>6</v>
       </c>
       <c r="R31" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S31" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T31" s="29" t="s">
-        <v>305</v>
+        <v>234</v>
+      </c>
+      <c r="T31" s="27" t="s">
+        <v>255</v>
       </c>
       <c r="U31" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>16</v>
       </c>
@@ -3567,12 +3606,12 @@
       <c r="D32" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="E32" s="30" t="s">
+      <c r="E32" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="F32" s="31"/>
-      <c r="G32" s="26" t="s">
-        <v>248</v>
+      <c r="F32" s="29"/>
+      <c r="G32" s="61" t="s">
+        <v>207</v>
       </c>
       <c r="H32" s="16">
         <v>30</v>
@@ -3580,8 +3619,8 @@
       <c r="I32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J32" s="32" t="s">
-        <v>249</v>
+      <c r="J32" s="59" t="s">
+        <v>208</v>
       </c>
       <c r="K32" s="5" t="s">
         <v>20</v>
@@ -3593,8 +3632,8 @@
         <v>59</v>
       </c>
       <c r="N32" s="6"/>
-      <c r="O32" s="31" t="s">
-        <v>272</v>
+      <c r="O32" s="29" t="s">
+        <v>222</v>
       </c>
       <c r="P32" s="16" t="s">
         <v>19</v>
@@ -3603,19 +3642,19 @@
         <v>6</v>
       </c>
       <c r="R32" s="20" t="s">
-        <v>298</v>
+        <v>248</v>
       </c>
       <c r="S32" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="T32" s="29" t="s">
-        <v>314</v>
+        <v>249</v>
+      </c>
+      <c r="T32" s="27" t="s">
+        <v>264</v>
       </c>
       <c r="U32" s="19" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>16</v>
       </c>
@@ -3628,12 +3667,12 @@
       <c r="D33" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="E33" s="30" t="s">
+      <c r="E33" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="F33" s="31"/>
-      <c r="G33" s="26" t="s">
-        <v>152</v>
+      <c r="F33" s="29"/>
+      <c r="G33" s="61" t="s">
+        <v>297</v>
       </c>
       <c r="H33" s="22">
         <v>31</v>
@@ -3641,8 +3680,8 @@
       <c r="I33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J33" s="32" t="s">
-        <v>251</v>
+      <c r="J33" s="59" t="s">
+        <v>324</v>
       </c>
       <c r="K33" s="5" t="s">
         <v>20</v>
@@ -3654,8 +3693,8 @@
       <c r="N33" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="O33" s="31" t="s">
-        <v>252</v>
+      <c r="O33" s="29" t="s">
+        <v>209</v>
       </c>
       <c r="P33" s="16" t="s">
         <v>19</v>
@@ -3664,19 +3703,19 @@
         <v>6</v>
       </c>
       <c r="R33" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S33" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T33" s="29" t="s">
-        <v>293</v>
+        <v>234</v>
+      </c>
+      <c r="T33" s="27" t="s">
+        <v>243</v>
       </c>
       <c r="U33" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>16</v>
       </c>
@@ -3689,12 +3728,12 @@
       <c r="D34" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="E34" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="F34" s="31"/>
-      <c r="G34" s="26" t="s">
-        <v>198</v>
+      <c r="F34" s="29"/>
+      <c r="G34" s="61" t="s">
+        <v>186</v>
       </c>
       <c r="H34" s="16">
         <v>32</v>
@@ -3702,8 +3741,8 @@
       <c r="I34" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J34" s="32" t="s">
-        <v>200</v>
+      <c r="J34" s="59" t="s">
+        <v>325</v>
       </c>
       <c r="K34" s="5" t="s">
         <v>19</v>
@@ -3713,8 +3752,8 @@
       </c>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
-      <c r="O34" s="31" t="s">
-        <v>319</v>
+      <c r="O34" s="29" t="s">
+        <v>269</v>
       </c>
       <c r="P34" s="16" t="s">
         <v>19</v>
@@ -3723,19 +3762,19 @@
         <v>9</v>
       </c>
       <c r="R34" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S34" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="T34" s="29" t="s">
-        <v>198</v>
+        <v>185</v>
+      </c>
+      <c r="T34" s="27" t="s">
+        <v>186</v>
       </c>
       <c r="U34" s="19" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>16</v>
       </c>
@@ -3748,12 +3787,12 @@
       <c r="D35" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="E35" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="F35" s="31"/>
-      <c r="G35" s="37" t="s">
-        <v>131</v>
+      <c r="F35" s="29"/>
+      <c r="G35" s="63" t="s">
+        <v>151</v>
       </c>
       <c r="H35" s="16">
         <v>33</v>
@@ -3761,8 +3800,8 @@
       <c r="I35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="32" t="s">
-        <v>253</v>
+      <c r="J35" s="59" t="s">
+        <v>210</v>
       </c>
       <c r="K35" s="5" t="s">
         <v>20</v>
@@ -3774,8 +3813,8 @@
         <v>64</v>
       </c>
       <c r="N35" s="6"/>
-      <c r="O35" s="31" t="s">
-        <v>320</v>
+      <c r="O35" s="29" t="s">
+        <v>270</v>
       </c>
       <c r="P35" s="16" t="s">
         <v>19</v>
@@ -3784,19 +3823,19 @@
         <v>6</v>
       </c>
       <c r="R35" s="20" t="s">
-        <v>298</v>
+        <v>248</v>
       </c>
       <c r="S35" s="19" t="s">
-        <v>299</v>
-      </c>
-      <c r="T35" s="29" t="s">
-        <v>315</v>
+        <v>249</v>
+      </c>
+      <c r="T35" s="27" t="s">
+        <v>265</v>
       </c>
       <c r="U35" s="19" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>16</v>
       </c>
@@ -3809,12 +3848,12 @@
       <c r="D36" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="E36" s="30" t="s">
+      <c r="E36" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="F36" s="31"/>
-      <c r="G36" s="26" t="s">
-        <v>273</v>
+      <c r="F36" s="29"/>
+      <c r="G36" s="61" t="s">
+        <v>223</v>
       </c>
       <c r="H36" s="22">
         <v>34</v>
@@ -3822,8 +3861,8 @@
       <c r="I36" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="32" t="s">
-        <v>254</v>
+      <c r="J36" s="59" t="s">
+        <v>211</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>20</v>
@@ -3835,8 +3874,8 @@
       <c r="N36" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="O36" s="31" t="s">
-        <v>274</v>
+      <c r="O36" s="29" t="s">
+        <v>224</v>
       </c>
       <c r="P36" s="16" t="s">
         <v>19</v>
@@ -3845,19 +3884,19 @@
         <v>6</v>
       </c>
       <c r="R36" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S36" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T36" s="29" t="s">
-        <v>294</v>
+        <v>234</v>
+      </c>
+      <c r="T36" s="27" t="s">
+        <v>244</v>
       </c>
       <c r="U36" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>16</v>
       </c>
@@ -3870,10 +3909,10 @@
       <c r="D37" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E37" s="30"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="26" t="s">
-        <v>255</v>
+      <c r="E37" s="28"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="61" t="s">
+        <v>298</v>
       </c>
       <c r="H37" s="16">
         <v>35</v>
@@ -3881,8 +3920,8 @@
       <c r="I37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J37" s="32" t="s">
-        <v>256</v>
+      <c r="J37" s="59" t="s">
+        <v>212</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>20</v>
@@ -3894,8 +3933,8 @@
       <c r="N37" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O37" s="31" t="s">
-        <v>279</v>
+      <c r="O37" s="29" t="s">
+        <v>229</v>
       </c>
       <c r="P37" s="16" t="s">
         <v>19</v>
@@ -3904,19 +3943,19 @@
         <v>6</v>
       </c>
       <c r="R37" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S37" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T37" s="29" t="s">
-        <v>296</v>
+        <v>234</v>
+      </c>
+      <c r="T37" s="27" t="s">
+        <v>246</v>
       </c>
       <c r="U37" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>16</v>
       </c>
@@ -3929,10 +3968,10 @@
       <c r="D38" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E38" s="30"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="26" t="s">
-        <v>258</v>
+      <c r="E38" s="28"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="61" t="s">
+        <v>213</v>
       </c>
       <c r="H38" s="16">
         <v>36</v>
@@ -3940,8 +3979,8 @@
       <c r="I38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J38" s="32" t="s">
-        <v>259</v>
+      <c r="J38" s="59" t="s">
+        <v>326</v>
       </c>
       <c r="K38" s="5" t="s">
         <v>20</v>
@@ -3953,8 +3992,8 @@
       <c r="N38" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O38" s="31" t="s">
-        <v>278</v>
+      <c r="O38" s="29" t="s">
+        <v>228</v>
       </c>
       <c r="P38" s="16" t="s">
         <v>19</v>
@@ -3963,19 +4002,19 @@
         <v>6</v>
       </c>
       <c r="R38" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S38" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T38" s="29" t="s">
-        <v>312</v>
+        <v>234</v>
+      </c>
+      <c r="T38" s="27" t="s">
+        <v>262</v>
       </c>
       <c r="U38" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>16</v>
       </c>
@@ -3988,10 +4027,10 @@
       <c r="D39" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E39" s="30"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="26" t="s">
-        <v>191</v>
+      <c r="E39" s="28"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="61" t="s">
+        <v>299</v>
       </c>
       <c r="H39" s="22">
         <v>37</v>
@@ -3999,8 +4038,8 @@
       <c r="I39" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J39" s="32" t="s">
-        <v>196</v>
+      <c r="J39" s="60" t="s">
+        <v>327</v>
       </c>
       <c r="K39" s="5" t="s">
         <v>20</v>
@@ -4010,8 +4049,8 @@
       </c>
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
-      <c r="O39" s="31" t="s">
-        <v>195</v>
+      <c r="O39" s="29" t="s">
+        <v>184</v>
       </c>
       <c r="P39" s="16" t="s">
         <v>19</v>
@@ -4020,19 +4059,19 @@
         <v>6</v>
       </c>
       <c r="R39" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="S39" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="T39" s="29" t="s">
-        <v>193</v>
+        <v>181</v>
+      </c>
+      <c r="T39" s="27" t="s">
+        <v>182</v>
       </c>
       <c r="U39" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>16</v>
       </c>
@@ -4045,10 +4084,10 @@
       <c r="D40" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E40" s="30"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="26" t="s">
-        <v>145</v>
+      <c r="E40" s="28"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="61" t="s">
+        <v>300</v>
       </c>
       <c r="H40" s="16">
         <v>38</v>
@@ -4056,8 +4095,8 @@
       <c r="I40" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J40" s="32" t="s">
-        <v>260</v>
+      <c r="J40" s="59" t="s">
+        <v>328</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>20</v>
@@ -4069,8 +4108,8 @@
       <c r="N40" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="O40" s="31" t="s">
-        <v>280</v>
+      <c r="O40" s="29" t="s">
+        <v>230</v>
       </c>
       <c r="P40" s="16" t="s">
         <v>19</v>
@@ -4079,19 +4118,19 @@
         <v>6</v>
       </c>
       <c r="R40" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S40" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T40" s="29" t="s">
-        <v>311</v>
+        <v>234</v>
+      </c>
+      <c r="T40" s="27" t="s">
+        <v>261</v>
       </c>
       <c r="U40" s="19" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>16</v>
       </c>
@@ -4104,10 +4143,10 @@
       <c r="D41" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="E41" s="30"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="26" t="s">
-        <v>153</v>
+      <c r="E41" s="28"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="61" t="s">
+        <v>301</v>
       </c>
       <c r="H41" s="16">
         <v>39</v>
@@ -4115,8 +4154,8 @@
       <c r="I41" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J41" s="32" t="s">
-        <v>257</v>
+      <c r="J41" s="59" t="s">
+        <v>329</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>20</v>
@@ -4128,8 +4167,8 @@
       <c r="N41" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="O41" s="31" t="s">
-        <v>261</v>
+      <c r="O41" s="29" t="s">
+        <v>214</v>
       </c>
       <c r="P41" s="16" t="s">
         <v>19</v>
@@ -4138,16 +4177,16 @@
         <v>6</v>
       </c>
       <c r="R41" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S41" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T41" s="29" t="s">
-        <v>306</v>
+        <v>234</v>
+      </c>
+      <c r="T41" s="27" t="s">
+        <v>256</v>
       </c>
       <c r="U41" s="19" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -4163,9 +4202,9 @@
       <c r="D42" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E42" s="30"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="26" t="s">
+      <c r="E42" s="28"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="61" t="s">
         <v>124</v>
       </c>
       <c r="H42" s="22">
@@ -4174,8 +4213,8 @@
       <c r="I42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J42" s="32" t="s">
-        <v>155</v>
+      <c r="J42" s="59" t="s">
+        <v>152</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>20</v>
@@ -4185,17 +4224,17 @@
       </c>
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
-      <c r="O42" s="31"/>
+      <c r="O42" s="29"/>
       <c r="P42" s="16" t="s">
         <v>19</v>
       </c>
       <c r="Q42" s="19"/>
       <c r="R42" s="20"/>
       <c r="S42" s="19"/>
-      <c r="T42" s="29"/>
+      <c r="T42" s="27"/>
       <c r="U42" s="19"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>16</v>
       </c>
@@ -4208,9 +4247,9 @@
       <c r="D43" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E43" s="30"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="38" t="s">
+      <c r="E43" s="28"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="64" t="s">
         <v>125</v>
       </c>
       <c r="H43" s="16">
@@ -4219,8 +4258,8 @@
       <c r="I43" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J43" s="32" t="s">
-        <v>156</v>
+      <c r="J43" s="59" t="s">
+        <v>153</v>
       </c>
       <c r="K43" s="5" t="s">
         <v>20</v>
@@ -4232,8 +4271,8 @@
       <c r="N43" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O43" s="31" t="s">
-        <v>158</v>
+      <c r="O43" s="29" t="s">
+        <v>155</v>
       </c>
       <c r="P43" s="16" t="s">
         <v>19</v>
@@ -4242,16 +4281,16 @@
         <v>6</v>
       </c>
       <c r="R43" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S43" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T43" s="29" t="s">
-        <v>303</v>
+        <v>234</v>
+      </c>
+      <c r="T43" s="27" t="s">
+        <v>253</v>
       </c>
       <c r="U43" s="19" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
@@ -4267,10 +4306,10 @@
       <c r="D44" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="E44" s="30"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="26" t="s">
-        <v>154</v>
+      <c r="E44" s="28"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="61" t="s">
+        <v>302</v>
       </c>
       <c r="H44" s="16">
         <v>42</v>
@@ -4278,8 +4317,8 @@
       <c r="I44" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J44" s="32" t="s">
-        <v>157</v>
+      <c r="J44" s="59" t="s">
+        <v>154</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>20</v>
@@ -4291,26 +4330,26 @@
       <c r="N44" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="O44" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="P44" s="16" t="s">
+      <c r="O44" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="P44" s="66" t="s">
         <v>20</v>
       </c>
       <c r="Q44" s="19">
         <v>6</v>
       </c>
       <c r="R44" s="20" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="S44" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="T44" s="29" t="s">
-        <v>313</v>
+        <v>234</v>
+      </c>
+      <c r="T44" s="27" t="s">
+        <v>263</v>
       </c>
       <c r="U44" s="19" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -6288,13 +6327,13 @@
       <c r="Q258" s="24"/>
     </row>
     <row r="266" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="P266" s="40"/>
-      <c r="Q266" s="40"/>
-      <c r="R266" s="40"/>
-      <c r="S266" s="40"/>
-      <c r="T266" s="40"/>
-      <c r="U266" s="40"/>
-      <c r="V266" s="40"/>
+      <c r="P266" s="33"/>
+      <c r="Q266" s="33"/>
+      <c r="R266" s="33"/>
+      <c r="S266" s="33"/>
+      <c r="T266" s="33"/>
+      <c r="U266" s="33"/>
+      <c r="V266" s="33"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:U2">

</xml_diff>

<commit_message>
Actualización de guion y escaleta guion 7
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/Escaleta_LE_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/Escaleta_LE_08_07_CO.xlsx
@@ -506,9 +506,6 @@
     <t>La oración simple: el sujeto y el predicado</t>
   </si>
   <si>
-    <t>Interactivo que realiza una presentación de los principales constituyentes de la oración: sujeto y predicado</t>
-  </si>
-  <si>
     <t>El análisis sintáctico</t>
   </si>
   <si>
@@ -624,9 +621,6 @@
   </si>
   <si>
     <t>6 preguntas que guíen al estudiante a identificar la intencionalidad de los ensayos.</t>
-  </si>
-  <si>
-    <t>Actividad para identificar las hipótesis de los ensayos</t>
   </si>
   <si>
     <t>6 imágenes acompañadas de preguntas que permitan inferir títulos de ensayos.</t>
@@ -861,9 +855,6 @@
     <t>Literatura: caracteriza el Realismo mágico</t>
   </si>
   <si>
-    <t>Gramática: identifica enlaces gramaticales</t>
-  </si>
-  <si>
     <t>Ortografía: reconoce los signos de puntuación</t>
   </si>
   <si>
@@ -873,9 +864,6 @@
     <t>Comprensión textual: el propósito de un ensayo</t>
   </si>
   <si>
-    <t>Producción textual: identifica títulos de ensayos</t>
-  </si>
-  <si>
     <t>Reconoce temas literarios</t>
   </si>
   <si>
@@ -949,22 +937,6 @@
   </si>
   <si>
     <t>Interactivo para distinguir el desarrollo literario de García Márquez</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Actividad para inferir ideas explicitas e implicitas en la obra </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cien años de soledad</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1031,9 +1003,6 @@
     <t xml:space="preserve">Interactivo que explica las partes de un ensayo </t>
   </si>
   <si>
-    <t>Actividad para distinguir las oraciones compuestas a partir del nexo</t>
-  </si>
-  <si>
     <t>Actividad para identificar la definición del guion, la raya y el paréntesis</t>
   </si>
   <si>
@@ -1041,6 +1010,37 @@
   </si>
   <si>
     <t>Actividad para reconocer las pautas para elaborar un ensayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gramática: identifica enlaces </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Producción textual: identifica títulos </t>
+  </si>
+  <si>
+    <t>Actividad para reconocer los titulos de ensayos a apartir de inferencias</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Actividad para inferir ideas explicitas e implícitas en la obra </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cien años de soledad</t>
+    </r>
+  </si>
+  <si>
+    <t>Interactivo que expone  los constituyentes de la oración: sujeto y predicado</t>
+  </si>
+  <si>
+    <t>Actividad para distinguir las oraciones compuestas a partir de los nexos</t>
   </si>
 </sst>
 </file>
@@ -1327,6 +1327,54 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1337,12 +1385,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1383,48 +1425,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1732,9 +1732,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P44" sqref="P44"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3:J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1763,94 +1763,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="56" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="G1" s="44" t="s">
+      <c r="F1" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="G1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="K1" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="50"/>
-      <c r="O1" s="38" t="s">
+      <c r="N1" s="64"/>
+      <c r="O1" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="38" t="s">
+      <c r="P1" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="53" t="s">
+      <c r="Q1" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="55" t="s">
+      <c r="T1" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="53" t="s">
+      <c r="U1" s="44" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="45"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="59"/>
       <c r="M2" s="25" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="54"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="45"/>
     </row>
     <row r="3" spans="1:21" ht="32.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -1867,8 +1867,8 @@
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="61" t="s">
-        <v>277</v>
+      <c r="G3" s="36" t="s">
+        <v>275</v>
       </c>
       <c r="H3" s="22">
         <v>1</v>
@@ -1876,8 +1876,8 @@
       <c r="I3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="65" t="s">
-        <v>303</v>
+      <c r="J3" s="40" t="s">
+        <v>299</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>20</v>
@@ -1890,7 +1890,7 @@
         <v>36</v>
       </c>
       <c r="O3" s="26" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="P3" s="15" t="s">
         <v>19</v>
@@ -1899,16 +1899,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T3" s="27" t="s">
         <v>233</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="U3" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T3" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="U3" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
@@ -1926,8 +1926,8 @@
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="61" t="s">
-        <v>278</v>
+      <c r="G4" s="36" t="s">
+        <v>324</v>
       </c>
       <c r="H4" s="16">
         <v>2</v>
@@ -1935,8 +1935,8 @@
       <c r="I4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="59" t="s">
-        <v>304</v>
+      <c r="J4" s="34" t="s">
+        <v>300</v>
       </c>
       <c r="K4" s="12" t="s">
         <v>20</v>
@@ -1949,7 +1949,7 @@
         <v>28</v>
       </c>
       <c r="O4" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P4" s="15" t="s">
         <v>19</v>
@@ -1958,16 +1958,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S4" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T4" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="U4" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T4" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="U4" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -1985,8 +1985,8 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="61" t="s">
-        <v>279</v>
+      <c r="G5" s="36" t="s">
+        <v>276</v>
       </c>
       <c r="H5" s="16">
         <v>3</v>
@@ -1994,8 +1994,8 @@
       <c r="I5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="59" t="s">
-        <v>226</v>
+      <c r="J5" s="34" t="s">
+        <v>224</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>20</v>
@@ -2008,7 +2008,7 @@
         <v>38</v>
       </c>
       <c r="O5" s="29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="P5" s="15" t="s">
         <v>19</v>
@@ -2017,16 +2017,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S5" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T5" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="U5" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T5" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="U5" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2044,8 +2044,8 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="29"/>
-      <c r="G6" s="61" t="s">
-        <v>280</v>
+      <c r="G6" s="36" t="s">
+        <v>277</v>
       </c>
       <c r="H6" s="22">
         <v>4</v>
@@ -2053,8 +2053,8 @@
       <c r="I6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="59" t="s">
-        <v>305</v>
+      <c r="J6" s="34" t="s">
+        <v>301</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>20</v>
@@ -2067,7 +2067,7 @@
         <v>24</v>
       </c>
       <c r="O6" s="29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P6" s="15" t="s">
         <v>19</v>
@@ -2076,16 +2076,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S6" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T6" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="U6" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T6" s="27" t="s">
-        <v>239</v>
-      </c>
-      <c r="U6" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2103,8 +2103,8 @@
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="29"/>
-      <c r="G7" s="61" t="s">
-        <v>281</v>
+      <c r="G7" s="36" t="s">
+        <v>278</v>
       </c>
       <c r="H7" s="16">
         <v>5</v>
@@ -2112,8 +2112,8 @@
       <c r="I7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="59" t="s">
-        <v>198</v>
+      <c r="J7" s="34" t="s">
+        <v>197</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>20</v>
@@ -2126,7 +2126,7 @@
         <v>120</v>
       </c>
       <c r="O7" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P7" s="15" t="s">
         <v>19</v>
@@ -2135,16 +2135,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S7" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T7" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="U7" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T7" s="27" t="s">
-        <v>240</v>
-      </c>
-      <c r="U7" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2162,8 +2162,8 @@
       </c>
       <c r="E8" s="28"/>
       <c r="F8" s="29"/>
-      <c r="G8" s="61" t="s">
-        <v>282</v>
+      <c r="G8" s="36" t="s">
+        <v>325</v>
       </c>
       <c r="H8" s="16">
         <v>6</v>
@@ -2171,8 +2171,8 @@
       <c r="I8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="59" t="s">
-        <v>200</v>
+      <c r="J8" s="34" t="s">
+        <v>326</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>20</v>
@@ -2185,7 +2185,7 @@
         <v>33</v>
       </c>
       <c r="O8" s="29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="P8" s="15" t="s">
         <v>19</v>
@@ -2194,16 +2194,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S8" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T8" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="U8" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T8" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="U8" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2220,11 +2220,11 @@
         <v>133</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F9" s="29"/>
-      <c r="G9" s="61" t="s">
-        <v>283</v>
+      <c r="G9" s="36" t="s">
+        <v>279</v>
       </c>
       <c r="H9" s="22">
         <v>7</v>
@@ -2232,8 +2232,8 @@
       <c r="I9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="59" t="s">
-        <v>306</v>
+      <c r="J9" s="34" t="s">
+        <v>302</v>
       </c>
       <c r="K9" s="12" t="s">
         <v>20</v>
@@ -2246,7 +2246,7 @@
         <v>36</v>
       </c>
       <c r="O9" s="29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>19</v>
@@ -2255,16 +2255,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S9" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T9" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="U9" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T9" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="U9" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2284,8 +2284,8 @@
         <v>134</v>
       </c>
       <c r="F10" s="29"/>
-      <c r="G10" s="61" t="s">
-        <v>284</v>
+      <c r="G10" s="36" t="s">
+        <v>280</v>
       </c>
       <c r="H10" s="16">
         <v>8</v>
@@ -2293,8 +2293,8 @@
       <c r="I10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="59" t="s">
-        <v>307</v>
+      <c r="J10" s="34" t="s">
+        <v>303</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>20</v>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="29" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="P10" s="15" t="s">
         <v>19</v>
@@ -2316,16 +2316,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="S10" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="T10" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="S10" s="19" t="s">
+      <c r="U10" s="19" t="s">
         <v>249</v>
-      </c>
-      <c r="T10" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="U10" s="19" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2345,8 +2345,8 @@
         <v>134</v>
       </c>
       <c r="F11" s="29"/>
-      <c r="G11" s="61" t="s">
-        <v>285</v>
+      <c r="G11" s="36" t="s">
+        <v>281</v>
       </c>
       <c r="H11" s="16">
         <v>9</v>
@@ -2354,8 +2354,8 @@
       <c r="I11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="59" t="s">
-        <v>308</v>
+      <c r="J11" s="34" t="s">
+        <v>327</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>20</v>
@@ -2368,7 +2368,7 @@
         <v>32</v>
       </c>
       <c r="O11" s="30" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="P11" s="15" t="s">
         <v>19</v>
@@ -2377,16 +2377,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S11" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T11" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="U11" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T11" s="27" t="s">
-        <v>252</v>
-      </c>
-      <c r="U11" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2406,8 +2406,8 @@
         <v>135</v>
       </c>
       <c r="F12" s="29"/>
-      <c r="G12" s="61" t="s">
-        <v>286</v>
+      <c r="G12" s="36" t="s">
+        <v>282</v>
       </c>
       <c r="H12" s="22">
         <v>10</v>
@@ -2415,8 +2415,8 @@
       <c r="I12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="59" t="s">
-        <v>309</v>
+      <c r="J12" s="34" t="s">
+        <v>304</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>20</v>
@@ -2429,25 +2429,25 @@
         <v>45</v>
       </c>
       <c r="O12" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="P12" s="66" t="s">
+        <v>230</v>
+      </c>
+      <c r="P12" s="41" t="s">
         <v>20</v>
       </c>
       <c r="Q12" s="19">
         <v>6</v>
       </c>
       <c r="R12" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S12" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T12" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="U12" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T12" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="U12" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2467,8 +2467,8 @@
         <v>136</v>
       </c>
       <c r="F13" s="29"/>
-      <c r="G13" s="61" t="s">
-        <v>287</v>
+      <c r="G13" s="36" t="s">
+        <v>283</v>
       </c>
       <c r="H13" s="16">
         <v>11</v>
@@ -2476,8 +2476,8 @@
       <c r="I13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="59" t="s">
-        <v>310</v>
+      <c r="J13" s="34" t="s">
+        <v>305</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>20</v>
@@ -2490,7 +2490,7 @@
         <v>37</v>
       </c>
       <c r="O13" s="29" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="P13" s="15" t="s">
         <v>19</v>
@@ -2499,16 +2499,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S13" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T13" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="U13" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T13" s="27" t="s">
-        <v>257</v>
-      </c>
-      <c r="U13" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2528,8 +2528,8 @@
         <v>121</v>
       </c>
       <c r="F14" s="29"/>
-      <c r="G14" s="61" t="s">
-        <v>196</v>
+      <c r="G14" s="36" t="s">
+        <v>195</v>
       </c>
       <c r="H14" s="16">
         <v>12</v>
@@ -2537,8 +2537,8 @@
       <c r="I14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="59" t="s">
-        <v>311</v>
+      <c r="J14" s="34" t="s">
+        <v>306</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>20</v>
@@ -2551,7 +2551,7 @@
         <v>120</v>
       </c>
       <c r="O14" s="29" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="P14" s="15" t="s">
         <v>19</v>
@@ -2560,16 +2560,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S14" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T14" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="U14" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T14" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="U14" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2589,7 +2589,7 @@
         <v>121</v>
       </c>
       <c r="F15" s="29"/>
-      <c r="G15" s="61" t="s">
+      <c r="G15" s="36" t="s">
         <v>129</v>
       </c>
       <c r="H15" s="22">
@@ -2598,8 +2598,8 @@
       <c r="I15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="59" t="s">
-        <v>312</v>
+      <c r="J15" s="34" t="s">
+        <v>307</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>20</v>
@@ -2612,7 +2612,7 @@
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="29" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="P15" s="15" t="s">
         <v>19</v>
@@ -2621,19 +2621,19 @@
         <v>6</v>
       </c>
       <c r="R15" s="20" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="S15" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="T15" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="U15" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="T15" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="U15" s="19" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>137</v>
       </c>
       <c r="F16" s="29"/>
-      <c r="G16" s="61" t="s">
+      <c r="G16" s="36" t="s">
         <v>159</v>
       </c>
       <c r="H16" s="16">
@@ -2659,8 +2659,8 @@
       <c r="I16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="59" t="s">
-        <v>160</v>
+      <c r="J16" s="34" t="s">
+        <v>328</v>
       </c>
       <c r="K16" s="5" t="s">
         <v>19</v>
@@ -2711,8 +2711,8 @@
       <c r="F17" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="G17" s="61" t="s">
-        <v>288</v>
+      <c r="G17" s="36" t="s">
+        <v>284</v>
       </c>
       <c r="H17" s="16">
         <v>15</v>
@@ -2720,8 +2720,8 @@
       <c r="I17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="59" t="s">
-        <v>313</v>
+      <c r="J17" s="34" t="s">
+        <v>308</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>20</v>
@@ -2734,7 +2734,7 @@
         <v>34</v>
       </c>
       <c r="O17" s="29" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="P17" s="16" t="s">
         <v>19</v>
@@ -2743,16 +2743,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S17" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T17" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="U17" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T17" s="27" t="s">
-        <v>273</v>
-      </c>
-      <c r="U17" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2772,8 +2772,8 @@
         <v>140</v>
       </c>
       <c r="F18" s="29"/>
-      <c r="G18" s="61" t="s">
-        <v>162</v>
+      <c r="G18" s="36" t="s">
+        <v>161</v>
       </c>
       <c r="H18" s="22">
         <v>16</v>
@@ -2781,8 +2781,8 @@
       <c r="I18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="59" t="s">
-        <v>314</v>
+      <c r="J18" s="34" t="s">
+        <v>309</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>19</v>
@@ -2805,13 +2805,13 @@
         <v>156</v>
       </c>
       <c r="S18" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="T18" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="T18" s="27" t="s">
+      <c r="U18" s="19" t="s">
         <v>162</v>
-      </c>
-      <c r="U18" s="19" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2831,8 +2831,8 @@
         <v>140</v>
       </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="61" t="s">
-        <v>167</v>
+      <c r="G19" s="36" t="s">
+        <v>166</v>
       </c>
       <c r="H19" s="16">
         <v>17</v>
@@ -2840,8 +2840,8 @@
       <c r="I19" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="59" t="s">
-        <v>168</v>
+      <c r="J19" s="34" t="s">
+        <v>167</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>19</v>
@@ -2864,13 +2864,13 @@
         <v>156</v>
       </c>
       <c r="S19" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="T19" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="T19" s="27" t="s">
+      <c r="U19" s="19" t="s">
         <v>170</v>
-      </c>
-      <c r="U19" s="19" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2892,8 +2892,8 @@
       <c r="F20" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="G20" s="61" t="s">
-        <v>289</v>
+      <c r="G20" s="36" t="s">
+        <v>285</v>
       </c>
       <c r="H20" s="16">
         <v>18</v>
@@ -2901,8 +2901,8 @@
       <c r="I20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="59" t="s">
-        <v>315</v>
+      <c r="J20" s="34" t="s">
+        <v>310</v>
       </c>
       <c r="K20" s="5" t="s">
         <v>20</v>
@@ -2915,7 +2915,7 @@
         <v>24</v>
       </c>
       <c r="O20" s="29" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="P20" s="16" t="s">
         <v>19</v>
@@ -2924,16 +2924,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S20" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T20" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="U20" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T20" s="27" t="s">
-        <v>276</v>
-      </c>
-      <c r="U20" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2953,8 +2953,8 @@
         <v>142</v>
       </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="61" t="s">
-        <v>290</v>
+      <c r="G21" s="36" t="s">
+        <v>286</v>
       </c>
       <c r="H21" s="22">
         <v>19</v>
@@ -2962,8 +2962,8 @@
       <c r="I21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="59" t="s">
-        <v>316</v>
+      <c r="J21" s="34" t="s">
+        <v>311</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>19</v>
@@ -2986,13 +2986,13 @@
         <v>156</v>
       </c>
       <c r="S21" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="T21" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="T21" s="27" t="s">
+      <c r="U21" s="19" t="s">
         <v>165</v>
-      </c>
-      <c r="U21" s="19" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3012,8 +3012,8 @@
         <v>122</v>
       </c>
       <c r="F22" s="29"/>
-      <c r="G22" s="62" t="s">
-        <v>291</v>
+      <c r="G22" s="37" t="s">
+        <v>287</v>
       </c>
       <c r="H22" s="16">
         <v>20</v>
@@ -3021,8 +3021,8 @@
       <c r="I22" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="60" t="s">
-        <v>317</v>
+      <c r="J22" s="35" t="s">
+        <v>312</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>19</v>
@@ -3035,7 +3035,7 @@
       <c r="O22" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="P22" s="66" t="s">
+      <c r="P22" s="41" t="s">
         <v>20</v>
       </c>
       <c r="Q22" s="19">
@@ -3045,13 +3045,13 @@
         <v>156</v>
       </c>
       <c r="S22" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="T22" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="T22" s="27" t="s">
+      <c r="U22" s="19" t="s">
         <v>173</v>
-      </c>
-      <c r="U22" s="19" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
@@ -3071,8 +3071,8 @@
         <v>122</v>
       </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="62" t="s">
-        <v>292</v>
+      <c r="G23" s="37" t="s">
+        <v>288</v>
       </c>
       <c r="H23" s="16">
         <v>21</v>
@@ -3080,8 +3080,8 @@
       <c r="I23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="60" t="s">
-        <v>318</v>
+      <c r="J23" s="35" t="s">
+        <v>313</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>19</v>
@@ -3094,7 +3094,7 @@
       <c r="O23" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="P23" s="66" t="s">
+      <c r="P23" s="41" t="s">
         <v>20</v>
       </c>
       <c r="Q23" s="19">
@@ -3107,10 +3107,10 @@
         <v>140</v>
       </c>
       <c r="T23" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="U23" s="19" t="s">
         <v>175</v>
-      </c>
-      <c r="U23" s="19" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3130,8 +3130,8 @@
         <v>122</v>
       </c>
       <c r="F24" s="29"/>
-      <c r="G24" s="62" t="s">
-        <v>204</v>
+      <c r="G24" s="37" t="s">
+        <v>202</v>
       </c>
       <c r="H24" s="22">
         <v>22</v>
@@ -3139,8 +3139,8 @@
       <c r="I24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="60" t="s">
-        <v>205</v>
+      <c r="J24" s="35" t="s">
+        <v>203</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>20</v>
@@ -3153,7 +3153,7 @@
         <v>120</v>
       </c>
       <c r="O24" s="29" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="P24" s="16" t="s">
         <v>19</v>
@@ -3162,16 +3162,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S24" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T24" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="U24" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T24" s="27" t="s">
-        <v>242</v>
-      </c>
-      <c r="U24" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3189,8 +3189,8 @@
       </c>
       <c r="E25" s="28"/>
       <c r="F25" s="29"/>
-      <c r="G25" s="62" t="s">
-        <v>177</v>
+      <c r="G25" s="37" t="s">
+        <v>176</v>
       </c>
       <c r="H25" s="16">
         <v>23</v>
@@ -3198,8 +3198,8 @@
       <c r="I25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J25" s="60" t="s">
-        <v>319</v>
+      <c r="J25" s="35" t="s">
+        <v>314</v>
       </c>
       <c r="K25" s="5" t="s">
         <v>19</v>
@@ -3222,13 +3222,13 @@
         <v>156</v>
       </c>
       <c r="S25" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="T25" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="U25" s="19" t="s">
         <v>178</v>
-      </c>
-      <c r="T25" s="27" t="s">
-        <v>177</v>
-      </c>
-      <c r="U25" s="19" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3248,8 +3248,8 @@
         <v>144</v>
       </c>
       <c r="F26" s="29"/>
-      <c r="G26" s="61" t="s">
-        <v>293</v>
+      <c r="G26" s="36" t="s">
+        <v>289</v>
       </c>
       <c r="H26" s="16">
         <v>24</v>
@@ -3257,8 +3257,8 @@
       <c r="I26" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="59" t="s">
-        <v>320</v>
+      <c r="J26" s="34" t="s">
+        <v>315</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>20</v>
@@ -3271,7 +3271,7 @@
         <v>27</v>
       </c>
       <c r="O26" s="29" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="P26" s="16" t="s">
         <v>19</v>
@@ -3280,16 +3280,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S26" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T26" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="U26" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T26" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="U26" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3306,11 +3306,11 @@
         <v>143</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="61" t="s">
-        <v>294</v>
+      <c r="G27" s="36" t="s">
+        <v>290</v>
       </c>
       <c r="H27" s="22">
         <v>25</v>
@@ -3318,8 +3318,8 @@
       <c r="I27" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="59" t="s">
-        <v>321</v>
+      <c r="J27" s="34" t="s">
+        <v>316</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>20</v>
@@ -3332,7 +3332,7 @@
         <v>36</v>
       </c>
       <c r="O27" s="29" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="P27" s="16" t="s">
         <v>19</v>
@@ -3341,16 +3341,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S27" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T27" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="U27" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T27" s="27" t="s">
-        <v>275</v>
-      </c>
-      <c r="U27" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3370,8 +3370,8 @@
         <v>122</v>
       </c>
       <c r="F28" s="29"/>
-      <c r="G28" s="61" t="s">
-        <v>295</v>
+      <c r="G28" s="36" t="s">
+        <v>291</v>
       </c>
       <c r="H28" s="16">
         <v>26</v>
@@ -3379,8 +3379,8 @@
       <c r="I28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="59" t="s">
-        <v>322</v>
+      <c r="J28" s="34" t="s">
+        <v>317</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>19</v>
@@ -3403,13 +3403,13 @@
         <v>156</v>
       </c>
       <c r="S28" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="T28" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="U28" s="19" t="s">
         <v>178</v>
-      </c>
-      <c r="T28" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="U28" s="19" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
@@ -3429,8 +3429,8 @@
         <v>122</v>
       </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="61" t="s">
-        <v>188</v>
+      <c r="G29" s="36" t="s">
+        <v>187</v>
       </c>
       <c r="H29" s="16">
         <v>27</v>
@@ -3438,8 +3438,8 @@
       <c r="I29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="59" t="s">
-        <v>323</v>
+      <c r="J29" s="34" t="s">
+        <v>318</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>19</v>
@@ -3462,13 +3462,13 @@
         <v>156</v>
       </c>
       <c r="S29" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="T29" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="T29" s="27" t="s">
+      <c r="U29" s="19" t="s">
         <v>190</v>
-      </c>
-      <c r="U29" s="19" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3488,8 +3488,8 @@
         <v>146</v>
       </c>
       <c r="F30" s="29"/>
-      <c r="G30" s="61" t="s">
-        <v>206</v>
+      <c r="G30" s="36" t="s">
+        <v>204</v>
       </c>
       <c r="H30" s="22">
         <v>28</v>
@@ -3497,8 +3497,8 @@
       <c r="I30" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J30" s="59" t="s">
-        <v>218</v>
+      <c r="J30" s="34" t="s">
+        <v>216</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>20</v>
@@ -3511,7 +3511,7 @@
         <v>28</v>
       </c>
       <c r="O30" s="29" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="P30" s="16" t="s">
         <v>19</v>
@@ -3520,16 +3520,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S30" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T30" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="U30" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T30" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="U30" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3549,8 +3549,8 @@
         <v>147</v>
       </c>
       <c r="F31" s="29"/>
-      <c r="G31" s="61" t="s">
-        <v>296</v>
+      <c r="G31" s="36" t="s">
+        <v>292</v>
       </c>
       <c r="H31" s="16">
         <v>29</v>
@@ -3558,8 +3558,8 @@
       <c r="I31" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="59" t="s">
-        <v>220</v>
+      <c r="J31" s="34" t="s">
+        <v>218</v>
       </c>
       <c r="K31" s="5" t="s">
         <v>20</v>
@@ -3572,7 +3572,7 @@
         <v>45</v>
       </c>
       <c r="O31" s="29" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="P31" s="16" t="s">
         <v>19</v>
@@ -3581,16 +3581,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S31" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T31" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="U31" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T31" s="27" t="s">
-        <v>255</v>
-      </c>
-      <c r="U31" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3610,8 +3610,8 @@
         <v>148</v>
       </c>
       <c r="F32" s="29"/>
-      <c r="G32" s="61" t="s">
-        <v>207</v>
+      <c r="G32" s="36" t="s">
+        <v>205</v>
       </c>
       <c r="H32" s="16">
         <v>30</v>
@@ -3619,8 +3619,8 @@
       <c r="I32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J32" s="59" t="s">
-        <v>208</v>
+      <c r="J32" s="34" t="s">
+        <v>206</v>
       </c>
       <c r="K32" s="5" t="s">
         <v>20</v>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="N32" s="6"/>
       <c r="O32" s="29" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="P32" s="16" t="s">
         <v>19</v>
@@ -3642,16 +3642,16 @@
         <v>6</v>
       </c>
       <c r="R32" s="20" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="S32" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="T32" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="U32" s="19" t="s">
         <v>249</v>
-      </c>
-      <c r="T32" s="27" t="s">
-        <v>264</v>
-      </c>
-      <c r="U32" s="19" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3671,8 +3671,8 @@
         <v>121</v>
       </c>
       <c r="F33" s="29"/>
-      <c r="G33" s="61" t="s">
-        <v>297</v>
+      <c r="G33" s="36" t="s">
+        <v>293</v>
       </c>
       <c r="H33" s="22">
         <v>31</v>
@@ -3680,8 +3680,8 @@
       <c r="I33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J33" s="59" t="s">
-        <v>324</v>
+      <c r="J33" s="34" t="s">
+        <v>319</v>
       </c>
       <c r="K33" s="5" t="s">
         <v>20</v>
@@ -3694,7 +3694,7 @@
         <v>120</v>
       </c>
       <c r="O33" s="29" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="P33" s="16" t="s">
         <v>19</v>
@@ -3703,16 +3703,16 @@
         <v>6</v>
       </c>
       <c r="R33" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S33" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T33" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="U33" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T33" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="U33" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3732,8 +3732,8 @@
         <v>150</v>
       </c>
       <c r="F34" s="29"/>
-      <c r="G34" s="61" t="s">
-        <v>186</v>
+      <c r="G34" s="36" t="s">
+        <v>185</v>
       </c>
       <c r="H34" s="16">
         <v>32</v>
@@ -3741,8 +3741,8 @@
       <c r="I34" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J34" s="59" t="s">
-        <v>325</v>
+      <c r="J34" s="34" t="s">
+        <v>320</v>
       </c>
       <c r="K34" s="5" t="s">
         <v>19</v>
@@ -3753,7 +3753,7 @@
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
       <c r="O34" s="29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="P34" s="16" t="s">
         <v>19</v>
@@ -3765,13 +3765,13 @@
         <v>156</v>
       </c>
       <c r="S34" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="T34" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="T34" s="27" t="s">
+      <c r="U34" s="19" t="s">
         <v>186</v>
-      </c>
-      <c r="U34" s="19" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3791,8 +3791,8 @@
         <v>151</v>
       </c>
       <c r="F35" s="29"/>
-      <c r="G35" s="63" t="s">
-        <v>151</v>
+      <c r="G35" s="38" t="s">
+        <v>131</v>
       </c>
       <c r="H35" s="16">
         <v>33</v>
@@ -3800,8 +3800,8 @@
       <c r="I35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J35" s="59" t="s">
-        <v>210</v>
+      <c r="J35" s="34" t="s">
+        <v>208</v>
       </c>
       <c r="K35" s="5" t="s">
         <v>20</v>
@@ -3814,7 +3814,7 @@
       </c>
       <c r="N35" s="6"/>
       <c r="O35" s="29" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="P35" s="16" t="s">
         <v>19</v>
@@ -3823,16 +3823,16 @@
         <v>6</v>
       </c>
       <c r="R35" s="20" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="S35" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="T35" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="U35" s="19" t="s">
         <v>249</v>
-      </c>
-      <c r="T35" s="27" t="s">
-        <v>265</v>
-      </c>
-      <c r="U35" s="19" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3852,8 +3852,8 @@
         <v>121</v>
       </c>
       <c r="F36" s="29"/>
-      <c r="G36" s="61" t="s">
-        <v>223</v>
+      <c r="G36" s="36" t="s">
+        <v>221</v>
       </c>
       <c r="H36" s="22">
         <v>34</v>
@@ -3861,8 +3861,8 @@
       <c r="I36" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="59" t="s">
-        <v>211</v>
+      <c r="J36" s="34" t="s">
+        <v>209</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>20</v>
@@ -3875,7 +3875,7 @@
         <v>120</v>
       </c>
       <c r="O36" s="29" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="P36" s="16" t="s">
         <v>19</v>
@@ -3884,16 +3884,16 @@
         <v>6</v>
       </c>
       <c r="R36" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S36" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T36" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="U36" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T36" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="U36" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3911,8 +3911,8 @@
       </c>
       <c r="E37" s="28"/>
       <c r="F37" s="29"/>
-      <c r="G37" s="61" t="s">
-        <v>298</v>
+      <c r="G37" s="36" t="s">
+        <v>294</v>
       </c>
       <c r="H37" s="16">
         <v>35</v>
@@ -3920,8 +3920,8 @@
       <c r="I37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J37" s="59" t="s">
-        <v>212</v>
+      <c r="J37" s="34" t="s">
+        <v>210</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>20</v>
@@ -3934,7 +3934,7 @@
         <v>33</v>
       </c>
       <c r="O37" s="29" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="P37" s="16" t="s">
         <v>19</v>
@@ -3943,16 +3943,16 @@
         <v>6</v>
       </c>
       <c r="R37" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S37" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T37" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="U37" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T37" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="U37" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3970,8 +3970,8 @@
       </c>
       <c r="E38" s="28"/>
       <c r="F38" s="29"/>
-      <c r="G38" s="61" t="s">
-        <v>213</v>
+      <c r="G38" s="36" t="s">
+        <v>211</v>
       </c>
       <c r="H38" s="16">
         <v>36</v>
@@ -3979,8 +3979,8 @@
       <c r="I38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J38" s="59" t="s">
-        <v>326</v>
+      <c r="J38" s="34" t="s">
+        <v>329</v>
       </c>
       <c r="K38" s="5" t="s">
         <v>20</v>
@@ -3993,7 +3993,7 @@
         <v>43</v>
       </c>
       <c r="O38" s="29" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="P38" s="16" t="s">
         <v>19</v>
@@ -4002,16 +4002,16 @@
         <v>6</v>
       </c>
       <c r="R38" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S38" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T38" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="U38" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T38" s="27" t="s">
-        <v>262</v>
-      </c>
-      <c r="U38" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -4029,8 +4029,8 @@
       </c>
       <c r="E39" s="28"/>
       <c r="F39" s="29"/>
-      <c r="G39" s="61" t="s">
-        <v>299</v>
+      <c r="G39" s="36" t="s">
+        <v>295</v>
       </c>
       <c r="H39" s="22">
         <v>37</v>
@@ -4038,8 +4038,8 @@
       <c r="I39" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J39" s="60" t="s">
-        <v>327</v>
+      <c r="J39" s="35" t="s">
+        <v>321</v>
       </c>
       <c r="K39" s="5" t="s">
         <v>20</v>
@@ -4050,7 +4050,7 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
       <c r="O39" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P39" s="16" t="s">
         <v>19</v>
@@ -4062,13 +4062,13 @@
         <v>156</v>
       </c>
       <c r="S39" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="T39" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="T39" s="27" t="s">
+      <c r="U39" s="19" t="s">
         <v>182</v>
-      </c>
-      <c r="U39" s="19" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -4086,8 +4086,8 @@
       </c>
       <c r="E40" s="28"/>
       <c r="F40" s="29"/>
-      <c r="G40" s="61" t="s">
-        <v>300</v>
+      <c r="G40" s="36" t="s">
+        <v>296</v>
       </c>
       <c r="H40" s="16">
         <v>38</v>
@@ -4095,8 +4095,8 @@
       <c r="I40" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J40" s="59" t="s">
-        <v>328</v>
+      <c r="J40" s="34" t="s">
+        <v>322</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>20</v>
@@ -4109,7 +4109,7 @@
         <v>28</v>
       </c>
       <c r="O40" s="29" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="P40" s="16" t="s">
         <v>19</v>
@@ -4118,16 +4118,16 @@
         <v>6</v>
       </c>
       <c r="R40" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S40" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T40" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="U40" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T40" s="27" t="s">
-        <v>261</v>
-      </c>
-      <c r="U40" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -4145,8 +4145,8 @@
       </c>
       <c r="E41" s="28"/>
       <c r="F41" s="29"/>
-      <c r="G41" s="61" t="s">
-        <v>301</v>
+      <c r="G41" s="36" t="s">
+        <v>297</v>
       </c>
       <c r="H41" s="16">
         <v>39</v>
@@ -4154,8 +4154,8 @@
       <c r="I41" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J41" s="59" t="s">
-        <v>329</v>
+      <c r="J41" s="34" t="s">
+        <v>323</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>20</v>
@@ -4168,7 +4168,7 @@
         <v>45</v>
       </c>
       <c r="O41" s="29" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="P41" s="16" t="s">
         <v>19</v>
@@ -4177,16 +4177,16 @@
         <v>6</v>
       </c>
       <c r="R41" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S41" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T41" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="U41" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T41" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="U41" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -4204,7 +4204,7 @@
       </c>
       <c r="E42" s="28"/>
       <c r="F42" s="29"/>
-      <c r="G42" s="61" t="s">
+      <c r="G42" s="36" t="s">
         <v>124</v>
       </c>
       <c r="H42" s="22">
@@ -4213,7 +4213,7 @@
       <c r="I42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J42" s="59" t="s">
+      <c r="J42" s="34" t="s">
         <v>152</v>
       </c>
       <c r="K42" s="5" t="s">
@@ -4249,7 +4249,7 @@
       </c>
       <c r="E43" s="28"/>
       <c r="F43" s="29"/>
-      <c r="G43" s="64" t="s">
+      <c r="G43" s="39" t="s">
         <v>125</v>
       </c>
       <c r="H43" s="16">
@@ -4258,7 +4258,7 @@
       <c r="I43" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J43" s="59" t="s">
+      <c r="J43" s="34" t="s">
         <v>153</v>
       </c>
       <c r="K43" s="5" t="s">
@@ -4281,16 +4281,16 @@
         <v>6</v>
       </c>
       <c r="R43" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S43" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T43" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="U43" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T43" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="U43" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
@@ -4308,8 +4308,8 @@
       </c>
       <c r="E44" s="28"/>
       <c r="F44" s="29"/>
-      <c r="G44" s="61" t="s">
-        <v>302</v>
+      <c r="G44" s="36" t="s">
+        <v>298</v>
       </c>
       <c r="H44" s="16">
         <v>42</v>
@@ -4317,7 +4317,7 @@
       <c r="I44" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J44" s="59" t="s">
+      <c r="J44" s="34" t="s">
         <v>154</v>
       </c>
       <c r="K44" s="5" t="s">
@@ -4331,25 +4331,25 @@
         <v>52</v>
       </c>
       <c r="O44" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="P44" s="66" t="s">
+        <v>193</v>
+      </c>
+      <c r="P44" s="41" t="s">
         <v>20</v>
       </c>
       <c r="Q44" s="19">
         <v>6</v>
       </c>
       <c r="R44" s="20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="S44" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T44" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="U44" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="T44" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="U44" s="19" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -6340,12 +6340,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -6360,6 +6354,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización de escaleta LE_08_07_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/Escaleta_LE_08_07_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion07/Escaleta_LE_08_07_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luz Amparo\Documents\GitHub\Lenguaje\fuentes\contenidos\grado08\guion07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AULA PLANETA\PROCESO JUNIO 2015\GRADO OCTAVO\LE_08_07_CO\Escaleta Proceso y control\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="329">
   <si>
     <t>Asignatura</t>
   </si>
@@ -488,9 +488,6 @@
     <t>Evalúa tus conocimientos sobre el tema El ensayo</t>
   </si>
   <si>
-    <t>Actividades sobre el tema El ensayo</t>
-  </si>
-  <si>
     <t>Realizar seis preguntas relacionadas con el tema El ensayo (temas vistos durante la unidad).</t>
   </si>
   <si>
@@ -648,12 +645,6 @@
   </si>
   <si>
     <t>8 preguntas relacionadas con los elementos, la estructura y las claves de un ensayo.</t>
-  </si>
-  <si>
-    <t>Interactivo para planear la escritura de un ensayo</t>
-  </si>
-  <si>
-    <t>Actividad para distinguir las pautas para escribir un ensayo</t>
   </si>
   <si>
     <t>Actividad para determinar el desarrollo de la novela en Colombia</t>
@@ -870,9 +861,6 @@
     <t xml:space="preserve">El sello literario de García Márquez </t>
   </si>
   <si>
-    <t>Comprende  la obra Cien años de soledad</t>
-  </si>
-  <si>
     <t>Determina la secuencia literaria</t>
   </si>
   <si>
@@ -891,9 +879,6 @@
     <t>Refuerza tu aprendizaje: Caracteriza las oraciones compuestas</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Ordena oraciones compuestas según el nexo</t>
-  </si>
-  <si>
     <t>Selecciona el signo ortográfico</t>
   </si>
   <si>
@@ -910,12 +895,6 @@
   </si>
   <si>
     <t>Literatura: la novela colombiana</t>
-  </si>
-  <si>
-    <t>Ortografía: define los signos de ortográficos</t>
-  </si>
-  <si>
-    <t>Comprensión textual: caracteriza un ensayo</t>
   </si>
   <si>
     <t>Producción textual: ordena los pasos de un ensayo</t>
@@ -997,18 +976,12 @@
     <t xml:space="preserve">Actividad para comprender la secuencia narrativa a partir de los signos de puntuación </t>
   </si>
   <si>
-    <t>Actividad para inferir ideas explícitas e implícitas en un ensayo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Interactivo que explica las partes de un ensayo </t>
   </si>
   <si>
     <t>Actividad para identificar la definición del guion, la raya y el paréntesis</t>
   </si>
   <si>
-    <t>Actividad para reconocer las características de un ensayo</t>
-  </si>
-  <si>
     <t>Actividad para reconocer las pautas para elaborar un ensayo</t>
   </si>
   <si>
@@ -1016,9 +989,6 @@
   </si>
   <si>
     <t xml:space="preserve">Producción textual: identifica títulos </t>
-  </si>
-  <si>
-    <t>Actividad para reconocer los titulos de ensayos a apartir de inferencias</t>
   </si>
   <si>
     <r>
@@ -1041,6 +1011,33 @@
   </si>
   <si>
     <t>Actividad para distinguir las oraciones compuestas a partir de los nexos</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer titulos de ensayos a apartir de inferencias</t>
+  </si>
+  <si>
+    <t>Comprende  la obra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: Ordena oraciones compuestas </t>
+  </si>
+  <si>
+    <t>Actividad paraidentificar ideas explícitas e inferir ideas implícitas en un ensayo</t>
+  </si>
+  <si>
+    <t>Interactivo para redactar un ensayo</t>
+  </si>
+  <si>
+    <t>Actividad para distinguir las elementos necesarios en la redacción de un ensayo</t>
+  </si>
+  <si>
+    <t>Ortografía: define los signos ortográficos</t>
+  </si>
+  <si>
+    <t>Actividad para reconocer la estructura de  un ensayo</t>
+  </si>
+  <si>
+    <t>Actividades para repasar los contenidos del tema El ensayo</t>
   </si>
 </sst>
 </file>
@@ -1351,30 +1348,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1385,6 +1358,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1424,6 +1403,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1732,9 +1729,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V266"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3:J44"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1763,94 +1760,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="50" t="s">
-        <v>223</v>
-      </c>
-      <c r="G1" s="58" t="s">
+      <c r="F1" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="G1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="K1" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="64"/>
-      <c r="O1" s="42" t="s">
+      <c r="N1" s="58"/>
+      <c r="O1" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="42" t="s">
+      <c r="P1" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="44" t="s">
+      <c r="Q1" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="R1" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="44" t="s">
+      <c r="S1" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="46" t="s">
+      <c r="T1" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="44" t="s">
+      <c r="U1" s="61" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="59"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="53"/>
       <c r="M2" s="25" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="45"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="32.25" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -1868,7 +1865,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="10"/>
       <c r="G3" s="36" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H3" s="22">
         <v>1</v>
@@ -1877,7 +1874,7 @@
         <v>20</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>20</v>
@@ -1890,7 +1887,7 @@
         <v>36</v>
       </c>
       <c r="O3" s="26" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="P3" s="15" t="s">
         <v>19</v>
@@ -1899,16 +1896,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S3" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T3" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="U3" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S3" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T3" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="U3" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
@@ -1927,7 +1924,7 @@
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
       <c r="G4" s="36" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="H4" s="16">
         <v>2</v>
@@ -1936,7 +1933,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="34" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="K4" s="12" t="s">
         <v>20</v>
@@ -1949,7 +1946,7 @@
         <v>28</v>
       </c>
       <c r="O4" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P4" s="15" t="s">
         <v>19</v>
@@ -1958,16 +1955,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S4" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T4" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="U4" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S4" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T4" s="27" t="s">
-        <v>235</v>
-      </c>
-      <c r="U4" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -1986,7 +1983,7 @@
       <c r="E5" s="28"/>
       <c r="F5" s="29"/>
       <c r="G5" s="36" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H5" s="16">
         <v>3</v>
@@ -1995,7 +1992,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="34" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>20</v>
@@ -2008,7 +2005,7 @@
         <v>38</v>
       </c>
       <c r="O5" s="29" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="P5" s="15" t="s">
         <v>19</v>
@@ -2017,16 +2014,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S5" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T5" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="U5" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S5" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T5" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="U5" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2045,7 +2042,7 @@
       <c r="E6" s="28"/>
       <c r="F6" s="29"/>
       <c r="G6" s="36" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H6" s="22">
         <v>4</v>
@@ -2054,7 +2051,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="34" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>20</v>
@@ -2067,7 +2064,7 @@
         <v>24</v>
       </c>
       <c r="O6" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P6" s="15" t="s">
         <v>19</v>
@@ -2076,16 +2073,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S6" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T6" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="U6" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S6" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T6" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="U6" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2104,7 +2101,7 @@
       <c r="E7" s="28"/>
       <c r="F7" s="29"/>
       <c r="G7" s="36" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H7" s="16">
         <v>5</v>
@@ -2113,7 +2110,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>20</v>
@@ -2126,7 +2123,7 @@
         <v>120</v>
       </c>
       <c r="O7" s="29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P7" s="15" t="s">
         <v>19</v>
@@ -2135,16 +2132,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S7" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T7" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="U7" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S7" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T7" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="U7" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2163,7 +2160,7 @@
       <c r="E8" s="28"/>
       <c r="F8" s="29"/>
       <c r="G8" s="36" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="H8" s="16">
         <v>6</v>
@@ -2172,7 +2169,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="34" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>20</v>
@@ -2185,7 +2182,7 @@
         <v>33</v>
       </c>
       <c r="O8" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P8" s="15" t="s">
         <v>19</v>
@@ -2194,16 +2191,16 @@
         <v>6</v>
       </c>
       <c r="R8" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S8" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T8" s="27" t="s">
+        <v>240</v>
+      </c>
+      <c r="U8" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S8" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T8" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="U8" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2220,11 +2217,11 @@
         <v>133</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="36" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H9" s="22">
         <v>7</v>
@@ -2233,7 +2230,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="K9" s="12" t="s">
         <v>20</v>
@@ -2246,7 +2243,7 @@
         <v>36</v>
       </c>
       <c r="O9" s="29" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>19</v>
@@ -2255,16 +2252,16 @@
         <v>6</v>
       </c>
       <c r="R9" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S9" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T9" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="U9" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S9" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T9" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="U9" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2285,7 +2282,7 @@
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="36" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H10" s="16">
         <v>8</v>
@@ -2294,7 +2291,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="34" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>20</v>
@@ -2307,7 +2304,7 @@
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="29" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="P10" s="15" t="s">
         <v>19</v>
@@ -2316,16 +2313,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="S10" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="T10" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="U10" s="19" t="s">
         <v>246</v>
-      </c>
-      <c r="S10" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="T10" s="27" t="s">
-        <v>248</v>
-      </c>
-      <c r="U10" s="19" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2346,7 +2343,7 @@
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="36" t="s">
-        <v>281</v>
+        <v>321</v>
       </c>
       <c r="H11" s="16">
         <v>9</v>
@@ -2355,7 +2352,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>20</v>
@@ -2368,7 +2365,7 @@
         <v>32</v>
       </c>
       <c r="O11" s="30" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="P11" s="15" t="s">
         <v>19</v>
@@ -2377,16 +2374,16 @@
         <v>6</v>
       </c>
       <c r="R11" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S11" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T11" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="U11" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S11" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T11" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="U11" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2407,7 +2404,7 @@
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="36" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="H12" s="22">
         <v>10</v>
@@ -2416,7 +2413,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="34" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="K12" s="12" t="s">
         <v>20</v>
@@ -2429,7 +2426,7 @@
         <v>45</v>
       </c>
       <c r="O12" s="29" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="P12" s="41" t="s">
         <v>20</v>
@@ -2438,16 +2435,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S12" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T12" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="U12" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S12" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T12" s="27" t="s">
-        <v>252</v>
-      </c>
-      <c r="U12" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2468,7 +2465,7 @@
       </c>
       <c r="F13" s="29"/>
       <c r="G13" s="36" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H13" s="16">
         <v>11</v>
@@ -2477,7 +2474,7 @@
         <v>19</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>20</v>
@@ -2490,7 +2487,7 @@
         <v>37</v>
       </c>
       <c r="O13" s="29" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="P13" s="15" t="s">
         <v>19</v>
@@ -2499,16 +2496,16 @@
         <v>6</v>
       </c>
       <c r="R13" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S13" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T13" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="U13" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S13" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T13" s="27" t="s">
-        <v>255</v>
-      </c>
-      <c r="U13" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2529,7 +2526,7 @@
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H14" s="16">
         <v>12</v>
@@ -2538,7 +2535,7 @@
         <v>19</v>
       </c>
       <c r="J14" s="34" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>20</v>
@@ -2551,7 +2548,7 @@
         <v>120</v>
       </c>
       <c r="O14" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P14" s="15" t="s">
         <v>19</v>
@@ -2560,16 +2557,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S14" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T14" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="U14" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S14" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T14" s="27" t="s">
-        <v>239</v>
-      </c>
-      <c r="U14" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2599,7 +2596,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="34" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>20</v>
@@ -2612,7 +2609,7 @@
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="29" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="P15" s="15" t="s">
         <v>19</v>
@@ -2621,16 +2618,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="S15" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="T15" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="U15" s="19" t="s">
         <v>246</v>
-      </c>
-      <c r="S15" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="T15" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="U15" s="19" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2651,7 +2648,7 @@
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H16" s="16">
         <v>14</v>
@@ -2660,7 +2657,7 @@
         <v>19</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="K16" s="5" t="s">
         <v>19</v>
@@ -2680,16 +2677,16 @@
         <v>8</v>
       </c>
       <c r="R16" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="S16" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="S16" s="19" t="s">
+      <c r="T16" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="U16" s="19" t="s">
         <v>157</v>
-      </c>
-      <c r="T16" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="U16" s="19" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2712,7 +2709,7 @@
         <v>138</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H17" s="16">
         <v>15</v>
@@ -2721,7 +2718,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="34" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>20</v>
@@ -2734,7 +2731,7 @@
         <v>34</v>
       </c>
       <c r="O17" s="29" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="P17" s="16" t="s">
         <v>19</v>
@@ -2743,16 +2740,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S17" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T17" s="27" t="s">
+        <v>268</v>
+      </c>
+      <c r="U17" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S17" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T17" s="27" t="s">
-        <v>271</v>
-      </c>
-      <c r="U17" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2773,7 +2770,7 @@
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H18" s="22">
         <v>16</v>
@@ -2782,7 +2779,7 @@
         <v>19</v>
       </c>
       <c r="J18" s="34" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>19</v>
@@ -2802,16 +2799,16 @@
         <v>10</v>
       </c>
       <c r="R18" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S18" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="T18" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="T18" s="27" t="s">
+      <c r="U18" s="19" t="s">
         <v>161</v>
-      </c>
-      <c r="U18" s="19" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2832,7 +2829,7 @@
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="36" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H19" s="16">
         <v>17</v>
@@ -2841,7 +2838,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K19" s="5" t="s">
         <v>19</v>
@@ -2861,16 +2858,16 @@
         <v>9</v>
       </c>
       <c r="R19" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S19" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="T19" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="T19" s="27" t="s">
+      <c r="U19" s="19" t="s">
         <v>169</v>
-      </c>
-      <c r="U19" s="19" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2893,7 +2890,7 @@
         <v>141</v>
       </c>
       <c r="G20" s="36" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="H20" s="16">
         <v>18</v>
@@ -2902,7 +2899,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="34" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="K20" s="5" t="s">
         <v>20</v>
@@ -2915,7 +2912,7 @@
         <v>24</v>
       </c>
       <c r="O20" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P20" s="16" t="s">
         <v>19</v>
@@ -2924,16 +2921,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S20" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T20" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="U20" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S20" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T20" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="U20" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -2954,7 +2951,7 @@
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="36" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="H21" s="22">
         <v>19</v>
@@ -2963,7 +2960,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="K21" s="5" t="s">
         <v>19</v>
@@ -2983,16 +2980,16 @@
         <v>10</v>
       </c>
       <c r="R21" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S21" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="T21" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="T21" s="27" t="s">
+      <c r="U21" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="U21" s="19" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3013,7 +3010,7 @@
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="37" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="H22" s="16">
         <v>20</v>
@@ -3022,7 +3019,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="35" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="K22" s="5" t="s">
         <v>19</v>
@@ -3042,16 +3039,16 @@
         <v>9</v>
       </c>
       <c r="R22" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S22" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="T22" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="T22" s="27" t="s">
+      <c r="U22" s="19" t="s">
         <v>172</v>
-      </c>
-      <c r="U22" s="19" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
@@ -3072,7 +3069,7 @@
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="37" t="s">
-        <v>288</v>
+        <v>322</v>
       </c>
       <c r="H23" s="16">
         <v>21</v>
@@ -3081,7 +3078,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="35" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="K23" s="5" t="s">
         <v>19</v>
@@ -3101,16 +3098,16 @@
         <v>9</v>
       </c>
       <c r="R23" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S23" s="19" t="s">
         <v>140</v>
       </c>
       <c r="T23" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="U23" s="19" t="s">
         <v>174</v>
-      </c>
-      <c r="U23" s="19" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3131,7 +3128,7 @@
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H24" s="22">
         <v>22</v>
@@ -3140,7 +3137,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="35" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K24" s="5" t="s">
         <v>20</v>
@@ -3153,7 +3150,7 @@
         <v>120</v>
       </c>
       <c r="O24" s="29" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="P24" s="16" t="s">
         <v>19</v>
@@ -3162,16 +3159,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S24" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T24" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="U24" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S24" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T24" s="27" t="s">
-        <v>240</v>
-      </c>
-      <c r="U24" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3190,7 +3187,7 @@
       <c r="E25" s="28"/>
       <c r="F25" s="29"/>
       <c r="G25" s="37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H25" s="16">
         <v>23</v>
@@ -3199,7 +3196,7 @@
         <v>19</v>
       </c>
       <c r="J25" s="35" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="K25" s="5" t="s">
         <v>19</v>
@@ -3219,16 +3216,16 @@
         <v>10</v>
       </c>
       <c r="R25" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S25" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="T25" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="U25" s="19" t="s">
         <v>177</v>
-      </c>
-      <c r="T25" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="U25" s="19" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3249,7 +3246,7 @@
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="36" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="H26" s="16">
         <v>24</v>
@@ -3258,7 +3255,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="34" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>20</v>
@@ -3271,7 +3268,7 @@
         <v>27</v>
       </c>
       <c r="O26" s="29" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="P26" s="16" t="s">
         <v>19</v>
@@ -3280,16 +3277,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S26" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T26" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="U26" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S26" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T26" s="27" t="s">
-        <v>257</v>
-      </c>
-      <c r="U26" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3306,11 +3303,11 @@
         <v>143</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F27" s="29"/>
       <c r="G27" s="36" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="H27" s="22">
         <v>25</v>
@@ -3319,7 +3316,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="34" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="K27" s="5" t="s">
         <v>20</v>
@@ -3332,7 +3329,7 @@
         <v>36</v>
       </c>
       <c r="O27" s="29" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P27" s="16" t="s">
         <v>19</v>
@@ -3341,16 +3338,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S27" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T27" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="U27" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S27" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T27" s="27" t="s">
-        <v>273</v>
-      </c>
-      <c r="U27" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3371,7 +3368,7 @@
       </c>
       <c r="F28" s="29"/>
       <c r="G28" s="36" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="H28" s="16">
         <v>26</v>
@@ -3380,7 +3377,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="34" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="K28" s="5" t="s">
         <v>19</v>
@@ -3400,16 +3397,16 @@
         <v>10</v>
       </c>
       <c r="R28" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S28" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="T28" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="U28" s="19" t="s">
         <v>177</v>
-      </c>
-      <c r="T28" s="27" t="s">
-        <v>179</v>
-      </c>
-      <c r="U28" s="19" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
@@ -3430,7 +3427,7 @@
       </c>
       <c r="F29" s="29"/>
       <c r="G29" s="36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H29" s="16">
         <v>27</v>
@@ -3439,7 +3436,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="34" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="K29" s="5" t="s">
         <v>19</v>
@@ -3459,16 +3456,16 @@
         <v>8</v>
       </c>
       <c r="R29" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S29" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="T29" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="T29" s="27" t="s">
+      <c r="U29" s="19" t="s">
         <v>189</v>
-      </c>
-      <c r="U29" s="19" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3489,7 +3486,7 @@
       </c>
       <c r="F30" s="29"/>
       <c r="G30" s="36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H30" s="22">
         <v>28</v>
@@ -3498,7 +3495,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="34" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>20</v>
@@ -3511,7 +3508,7 @@
         <v>28</v>
       </c>
       <c r="O30" s="29" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="P30" s="16" t="s">
         <v>19</v>
@@ -3520,16 +3517,16 @@
         <v>6</v>
       </c>
       <c r="R30" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S30" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T30" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="U30" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S30" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T30" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="U30" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3550,7 +3547,7 @@
       </c>
       <c r="F31" s="29"/>
       <c r="G31" s="36" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H31" s="16">
         <v>29</v>
@@ -3559,7 +3556,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="34" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K31" s="5" t="s">
         <v>20</v>
@@ -3572,7 +3569,7 @@
         <v>45</v>
       </c>
       <c r="O31" s="29" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="P31" s="16" t="s">
         <v>19</v>
@@ -3581,16 +3578,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S31" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T31" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="U31" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S31" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T31" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="U31" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3611,7 +3608,7 @@
       </c>
       <c r="F32" s="29"/>
       <c r="G32" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H32" s="16">
         <v>30</v>
@@ -3620,7 +3617,7 @@
         <v>19</v>
       </c>
       <c r="J32" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K32" s="5" t="s">
         <v>20</v>
@@ -3633,7 +3630,7 @@
       </c>
       <c r="N32" s="6"/>
       <c r="O32" s="29" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="P32" s="16" t="s">
         <v>19</v>
@@ -3642,16 +3639,16 @@
         <v>6</v>
       </c>
       <c r="R32" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="S32" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="T32" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="U32" s="19" t="s">
         <v>246</v>
-      </c>
-      <c r="S32" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="T32" s="27" t="s">
-        <v>262</v>
-      </c>
-      <c r="U32" s="19" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3672,7 +3669,7 @@
       </c>
       <c r="F33" s="29"/>
       <c r="G33" s="36" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="H33" s="22">
         <v>31</v>
@@ -3681,7 +3678,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="34" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="K33" s="5" t="s">
         <v>20</v>
@@ -3694,7 +3691,7 @@
         <v>120</v>
       </c>
       <c r="O33" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="P33" s="16" t="s">
         <v>19</v>
@@ -3703,16 +3700,16 @@
         <v>6</v>
       </c>
       <c r="R33" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S33" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T33" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="U33" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S33" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T33" s="27" t="s">
-        <v>241</v>
-      </c>
-      <c r="U33" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3733,7 +3730,7 @@
       </c>
       <c r="F34" s="29"/>
       <c r="G34" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H34" s="16">
         <v>32</v>
@@ -3742,7 +3739,7 @@
         <v>19</v>
       </c>
       <c r="J34" s="34" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="K34" s="5" t="s">
         <v>19</v>
@@ -3753,7 +3750,7 @@
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
       <c r="O34" s="29" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="P34" s="16" t="s">
         <v>19</v>
@@ -3762,19 +3759,19 @@
         <v>9</v>
       </c>
       <c r="R34" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S34" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="T34" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="T34" s="27" t="s">
+      <c r="U34" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="U34" s="19" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>16</v>
       </c>
@@ -3792,7 +3789,7 @@
       </c>
       <c r="F35" s="29"/>
       <c r="G35" s="38" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="H35" s="16">
         <v>33</v>
@@ -3801,7 +3798,7 @@
         <v>19</v>
       </c>
       <c r="J35" s="34" t="s">
-        <v>208</v>
+        <v>324</v>
       </c>
       <c r="K35" s="5" t="s">
         <v>20</v>
@@ -3814,7 +3811,7 @@
       </c>
       <c r="N35" s="6"/>
       <c r="O35" s="29" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="P35" s="16" t="s">
         <v>19</v>
@@ -3823,16 +3820,16 @@
         <v>6</v>
       </c>
       <c r="R35" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="S35" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="T35" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="U35" s="19" t="s">
         <v>246</v>
-      </c>
-      <c r="S35" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="T35" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="U35" s="19" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3853,7 +3850,7 @@
       </c>
       <c r="F36" s="29"/>
       <c r="G36" s="36" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H36" s="22">
         <v>34</v>
@@ -3862,7 +3859,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="34" t="s">
-        <v>209</v>
+        <v>325</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>20</v>
@@ -3875,7 +3872,7 @@
         <v>120</v>
       </c>
       <c r="O36" s="29" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P36" s="16" t="s">
         <v>19</v>
@@ -3884,16 +3881,16 @@
         <v>6</v>
       </c>
       <c r="R36" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S36" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T36" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="U36" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S36" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T36" s="27" t="s">
-        <v>242</v>
-      </c>
-      <c r="U36" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3912,7 +3909,7 @@
       <c r="E37" s="28"/>
       <c r="F37" s="29"/>
       <c r="G37" s="36" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H37" s="16">
         <v>35</v>
@@ -3921,7 +3918,7 @@
         <v>20</v>
       </c>
       <c r="J37" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K37" s="5" t="s">
         <v>20</v>
@@ -3934,7 +3931,7 @@
         <v>33</v>
       </c>
       <c r="O37" s="29" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="P37" s="16" t="s">
         <v>19</v>
@@ -3943,16 +3940,16 @@
         <v>6</v>
       </c>
       <c r="R37" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S37" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T37" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="U37" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S37" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T37" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="U37" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -3971,7 +3968,7 @@
       <c r="E38" s="28"/>
       <c r="F38" s="29"/>
       <c r="G38" s="36" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H38" s="16">
         <v>36</v>
@@ -3980,7 +3977,7 @@
         <v>20</v>
       </c>
       <c r="J38" s="34" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="K38" s="5" t="s">
         <v>20</v>
@@ -3993,7 +3990,7 @@
         <v>43</v>
       </c>
       <c r="O38" s="29" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="P38" s="16" t="s">
         <v>19</v>
@@ -4002,16 +3999,16 @@
         <v>6</v>
       </c>
       <c r="R38" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S38" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T38" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="U38" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S38" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T38" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="U38" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -4030,7 +4027,7 @@
       <c r="E39" s="28"/>
       <c r="F39" s="29"/>
       <c r="G39" s="36" t="s">
-        <v>295</v>
+        <v>326</v>
       </c>
       <c r="H39" s="22">
         <v>37</v>
@@ -4039,7 +4036,7 @@
         <v>20</v>
       </c>
       <c r="J39" s="35" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="K39" s="5" t="s">
         <v>20</v>
@@ -4050,7 +4047,7 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
       <c r="O39" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P39" s="16" t="s">
         <v>19</v>
@@ -4059,16 +4056,16 @@
         <v>6</v>
       </c>
       <c r="R39" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S39" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="T39" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="T39" s="27" t="s">
+      <c r="U39" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="U39" s="19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -4087,7 +4084,7 @@
       <c r="E40" s="28"/>
       <c r="F40" s="29"/>
       <c r="G40" s="36" t="s">
-        <v>296</v>
+        <v>145</v>
       </c>
       <c r="H40" s="16">
         <v>38</v>
@@ -4096,7 +4093,7 @@
         <v>20</v>
       </c>
       <c r="J40" s="34" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>20</v>
@@ -4109,7 +4106,7 @@
         <v>28</v>
       </c>
       <c r="O40" s="29" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="P40" s="16" t="s">
         <v>19</v>
@@ -4118,16 +4115,16 @@
         <v>6</v>
       </c>
       <c r="R40" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S40" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T40" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="U40" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S40" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T40" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="U40" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
@@ -4146,7 +4143,7 @@
       <c r="E41" s="28"/>
       <c r="F41" s="29"/>
       <c r="G41" s="36" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="H41" s="16">
         <v>39</v>
@@ -4155,7 +4152,7 @@
         <v>20</v>
       </c>
       <c r="J41" s="34" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>20</v>
@@ -4168,7 +4165,7 @@
         <v>45</v>
       </c>
       <c r="O41" s="29" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P41" s="16" t="s">
         <v>19</v>
@@ -4177,16 +4174,16 @@
         <v>6</v>
       </c>
       <c r="R41" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S41" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T41" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="U41" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S41" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T41" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="U41" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -4272,7 +4269,7 @@
         <v>32</v>
       </c>
       <c r="O43" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P43" s="16" t="s">
         <v>19</v>
@@ -4281,19 +4278,19 @@
         <v>6</v>
       </c>
       <c r="R43" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S43" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T43" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="U43" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="S43" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T43" s="27" t="s">
-        <v>251</v>
-      </c>
-      <c r="U43" s="19" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>16</v>
       </c>
@@ -4309,7 +4306,7 @@
       <c r="E44" s="28"/>
       <c r="F44" s="29"/>
       <c r="G44" s="36" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="H44" s="16">
         <v>42</v>
@@ -4318,7 +4315,7 @@
         <v>20</v>
       </c>
       <c r="J44" s="34" t="s">
-        <v>154</v>
+        <v>328</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>20</v>
@@ -4331,7 +4328,7 @@
         <v>52</v>
       </c>
       <c r="O44" s="29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P44" s="41" t="s">
         <v>20</v>
@@ -4340,16 +4337,16 @@
         <v>6</v>
       </c>
       <c r="R44" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="S44" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="T44" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="U44" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="S44" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="T44" s="27" t="s">
-        <v>261</v>
-      </c>
-      <c r="U44" s="19" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -6340,6 +6337,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -6354,12 +6357,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>